<commit_message>
Excel da T3 - 100% finalizado
</commit_message>
<xml_diff>
--- a/EXP 3/T3.xlsx
+++ b/EXP 3/T3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAIII\EXP 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D432D9-2B93-4F22-B566-3BAAB5CA0101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8D89A3-970F-44FF-99C3-36625C0D0F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CAF38A1F-BD9D-416B-BE17-8DE3D13292B8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{CAF38A1F-BD9D-416B-BE17-8DE3D13292B8}"/>
   </bookViews>
   <sheets>
     <sheet name="P1.1" sheetId="1" r:id="rId1"/>
@@ -41,8 +41,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
   <si>
     <t>Determinação do n do ar - Método 1</t>
   </si>
@@ -484,23 +506,127 @@
       <t>) (%)</t>
     </r>
   </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Média de N</t>
+  </si>
+  <si>
+    <t>u(Média de N)</t>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>v</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> médio</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>u(n</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> médio)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>u(n</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> médio) (%)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.0000%"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.0E+00"/>
-    <numFmt numFmtId="172" formatCode="0E+00"/>
-    <numFmt numFmtId="173" formatCode="0.000E+00"/>
-    <numFmt numFmtId="175" formatCode="0.000%"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="0.0E+00"/>
+    <numFmt numFmtId="170" formatCode="0E+00"/>
+    <numFmt numFmtId="171" formatCode="0.000E+00"/>
+    <numFmt numFmtId="174" formatCode="0.000000"/>
+    <numFmt numFmtId="175" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,6 +666,21 @@
       <vertAlign val="subscript"/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -678,7 +819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -698,9 +839,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -713,49 +851,22 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -767,13 +878,16 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -785,7 +899,58 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -806,6 +971,353 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'P1.1'!$E$7:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'P1.1'!$C$7:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>77.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>111.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5CEA-4EB3-AA95-B8FFD33AA671}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="275577712"/>
+        <c:axId val="1988631632"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="275577712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1988631632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1988631632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="275577712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1424,7 +1936,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1957,7 +2469,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1990,9 +2502,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>N(p)</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -2143,6 +2652,13 @@
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:v>N(p)</c:v>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-49EE-4463-99F7-959DF4B2D737}"/>
             </c:ext>
@@ -2151,9 +2667,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>ajuste</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:solidFill>
@@ -2318,6 +2831,13 @@
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:v>ajuste</c:v>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-49EE-4463-99F7-959DF4B2D737}"/>
             </c:ext>
@@ -2620,7 +3140,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3160,7 +3680,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3320,7 +3840,7 @@
                   <c:v>1.7999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.35E-2</c:v>
+                  <c:v>2.5499999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.7E-2</c:v>
@@ -3528,7 +4048,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3888,7 +4408,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4224,7 +4744,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4379,7 +4899,7 @@
                   <c:v>1.7999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.35E-2</c:v>
+                  <c:v>2.5499999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.7E-2</c:v>
@@ -4984,6 +5504,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -8597,6 +9157,522 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9156,6 +10232,42 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34387A32-126D-F877-18B6-6465CDDFE4C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -9540,14 +10652,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>238206</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>417</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1986</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -9572,8 +10684,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9700260" y="366177"/>
-          <a:ext cx="4030980" cy="883503"/>
+          <a:off x="9627371" y="371478"/>
+          <a:ext cx="4030980" cy="894105"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10094,59 +11206,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0D8ADF-2EFB-452A-A480-0B215EA5BBF1}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.88671875" style="1" customWidth="1"/>
-    <col min="3" max="12" width="8.88671875" style="1"/>
+    <col min="3" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="8.88671875" style="1"/>
     <col min="13" max="13" width="14" style="1" customWidth="1"/>
     <col min="14" max="14" width="9.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -10181,34 +11296,34 @@
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="13">
         <v>12</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="13">
         <v>10.5</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="13">
         <v>11.5</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="13">
         <v>10.7</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="13">
         <v>11.3</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="13">
         <v>10</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="13">
         <v>11.1</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="13">
         <v>11</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="13">
         <v>12</v>
       </c>
-      <c r="K4" s="19">
+      <c r="K4" s="13">
         <v>11</v>
       </c>
       <c r="M4" s="2" t="s">
@@ -10265,7 +11380,7 @@
       <c r="M5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="22">
+      <c r="N5" s="16">
         <v>6.328E-7</v>
       </c>
     </row>
@@ -10278,9 +11393,38 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="E7" s="7"/>
+      <c r="B7" s="13">
+        <f>B4</f>
+        <v>12</v>
+      </c>
+      <c r="C7" s="35">
+        <f>B7</f>
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
+        <f>C7*10^-6</f>
+        <v>1.2E-5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B8" s="13">
+        <f>C4</f>
+        <v>10.5</v>
+      </c>
+      <c r="C8" s="35">
+        <f>C7+B8</f>
+        <v>22.5</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" ref="D8:D16" si="1">C8*10^-6</f>
+        <v>2.2499999999999998E-5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>60</v>
+      </c>
       <c r="M8" s="2" t="s">
         <v>5</v>
       </c>
@@ -10289,6 +11433,27 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B9" s="13">
+        <v>11.5</v>
+      </c>
+      <c r="C9" s="35">
+        <f>C8+B9</f>
+        <v>34</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="1"/>
+        <v>3.4E-5</v>
+      </c>
+      <c r="E9" s="1">
+        <v>90</v>
+      </c>
+      <c r="G9" s="1" cm="1">
+        <f t="array" ref="G9:H13">LINEST(D7:D16,E7:E16,1,1)</f>
+        <v>3.6622222222222229E-7</v>
+      </c>
+      <c r="H9" s="1">
+        <v>7.3333333333331502E-7</v>
+      </c>
       <c r="M9" s="2" t="s">
         <v>54</v>
       </c>
@@ -10298,33 +11463,113 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="13">
+        <v>10.7</v>
+      </c>
+      <c r="C10" s="35">
+        <f t="shared" ref="C10:C16" si="2">C9+B10</f>
+        <v>44.7</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="1"/>
+        <v>4.4700000000000002E-5</v>
+      </c>
+      <c r="E10" s="1">
+        <v>120</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1.7452838487427891E-9</v>
+      </c>
+      <c r="H10" s="1">
+        <v>3.2487604473775323E-7</v>
+      </c>
       <c r="M10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="15">
         <f>_xlfn.STDEV.P(B5:K5)/SQRT(10)</f>
         <v>1.8891797161731345E-7</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="13">
+        <v>11.3</v>
+      </c>
+      <c r="C11" s="35">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="1"/>
+        <v>5.5999999999999999E-5</v>
+      </c>
+      <c r="E11" s="1">
+        <v>150</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.99981834228837585</v>
+      </c>
+      <c r="H11" s="1">
+        <v>4.7556983363820639E-7</v>
+      </c>
       <c r="M11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="7">
         <f>(N8*$N$5)/(2*N9)</f>
         <v>0.85436543654365449</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="13">
+        <v>10</v>
+      </c>
+      <c r="C12" s="35">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="1"/>
+        <v>6.5999999999999992E-5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>180</v>
+      </c>
+      <c r="G12" s="1">
+        <v>44030.868091377131</v>
+      </c>
+      <c r="H12" s="1">
+        <v>8</v>
+      </c>
       <c r="M12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="7">
         <f>ABS(N8*2/((2*N9)^2)*N5*N10)</f>
         <v>1.4527901466405738E-2</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B13" s="13">
+        <v>11.1</v>
+      </c>
+      <c r="C13" s="35">
+        <f t="shared" si="2"/>
+        <v>77.099999999999994</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="1"/>
+        <v>7.709999999999999E-5</v>
+      </c>
+      <c r="E13" s="1">
+        <v>210</v>
+      </c>
+      <c r="G13" s="1">
+        <v>9.9583146666666644E-9</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1.8093333333333703E-12</v>
+      </c>
       <c r="M13" s="2" t="s">
         <v>34</v>
       </c>
@@ -10334,12 +11579,65 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="13">
+        <v>11</v>
+      </c>
+      <c r="C14" s="35">
+        <f t="shared" si="2"/>
+        <v>88.1</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="1"/>
+        <v>8.8099999999999987E-5</v>
+      </c>
+      <c r="E14" s="1">
+        <v>240</v>
+      </c>
       <c r="M14" s="2" t="s">
         <v>50</v>
       </c>
       <c r="N14" s="6">
         <f>ABS(N11-N6)/N6</f>
         <v>0.14588225760164095</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B15" s="13">
+        <v>12</v>
+      </c>
+      <c r="C15" s="35">
+        <f t="shared" si="2"/>
+        <v>100.1</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0009999999999999E-4</v>
+      </c>
+      <c r="E15" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B16" s="13">
+        <v>11</v>
+      </c>
+      <c r="C16" s="35">
+        <f t="shared" si="2"/>
+        <v>111.1</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1109999999999999E-4</v>
+      </c>
+      <c r="E16" s="1">
+        <v>300</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="36">
+        <f>N5/(2*G9)</f>
+        <v>0.86395631067961154</v>
       </c>
     </row>
   </sheetData>
@@ -10356,102 +11654,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A1DA6F-08FA-487A-82B4-E9BF2212A846}">
   <dimension ref="A1:AM23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG15" sqref="AG15"/>
+    <sheetView topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AK12" sqref="AK12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="10" width="8.88671875" style="1"/>
     <col min="11" max="11" width="12.21875" style="1" customWidth="1"/>
-    <col min="12" max="28" width="8.88671875" style="1"/>
+    <col min="12" max="27" width="8.88671875" style="1"/>
+    <col min="28" max="28" width="13" style="1" customWidth="1"/>
     <col min="29" max="29" width="8.88671875" style="1" customWidth="1"/>
     <col min="30" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="20"/>
+      <c r="AG1" s="20"/>
+      <c r="AH1" s="20"/>
+      <c r="AI1" s="20"/>
+      <c r="AJ1" s="20"/>
+      <c r="AK1" s="20"/>
+      <c r="AL1" s="20"/>
+      <c r="AM1" s="20"/>
     </row>
     <row r="2" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="13"/>
-      <c r="AF2" s="13"/>
-      <c r="AG2" s="13"/>
-      <c r="AH2" s="13"/>
-      <c r="AI2" s="13"/>
-      <c r="AJ2" s="13"/>
-      <c r="AK2" s="13"/>
-      <c r="AL2" s="13"/>
-      <c r="AM2" s="13"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="20"/>
+      <c r="AL2" s="20"/>
+      <c r="AM2" s="20"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -10482,7 +11781,7 @@
         <v>5</v>
       </c>
       <c r="AC3" s="3">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="AD3" s="3">
         <v>23</v>
@@ -10519,25 +11818,25 @@
       <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="9">
-        <f>A4*G$21+H$21</f>
+      <c r="C4" s="8">
+        <f t="shared" ref="C4:C19" si="0">A4*G$21+H$21</f>
         <v>1.8435076018527372</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <f>B4-C4</f>
         <v>1.1564923981472628</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="13">
         <v>0.3</v>
       </c>
       <c r="O4" s="3">
         <v>5</v>
       </c>
-      <c r="P4" s="9">
-        <f>N4*T$21+U$21</f>
+      <c r="P4" s="8">
+        <f t="shared" ref="P4:P21" si="1">N4*T$21+U$21</f>
         <v>4.730994152046792</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="Q4" s="8">
         <f>O4-P4</f>
         <v>0.26900584795320803</v>
       </c>
@@ -10549,34 +11848,34 @@
       <c r="B5" s="3">
         <v>5</v>
       </c>
-      <c r="C5" s="9">
-        <f>A5*G$21+H$21</f>
+      <c r="C5" s="8">
+        <f t="shared" si="0"/>
         <v>4.9247170363203114</v>
       </c>
-      <c r="D5" s="9">
-        <f t="shared" ref="D5:D19" si="0">B5-C5</f>
+      <c r="D5" s="8">
+        <f t="shared" ref="D5:D19" si="2">B5-C5</f>
         <v>7.5282963679688564E-2</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="13">
         <v>0.4</v>
       </c>
       <c r="O5" s="3">
         <v>8</v>
       </c>
-      <c r="P5" s="9">
-        <f>N5*T$21+U$21</f>
+      <c r="P5" s="8">
+        <f t="shared" si="1"/>
         <v>7.0436876504988035</v>
       </c>
-      <c r="Q5" s="9">
-        <f t="shared" ref="Q5:Q21" si="1">O5-P5</f>
+      <c r="Q5" s="8">
+        <f t="shared" ref="Q5:Q21" si="3">O5-P5</f>
         <v>0.95631234950119648</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="AC5" s="3">
         <f>AVERAGE(AC3:AL3)</f>
-        <v>20.3</v>
+        <v>20.6</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.3">
@@ -10586,34 +11885,34 @@
       <c r="B6" s="3">
         <v>8</v>
       </c>
-      <c r="C6" s="9">
-        <f>A6*G$21+H$21</f>
+      <c r="C6" s="8">
+        <f t="shared" si="0"/>
         <v>8.0059264707878839</v>
       </c>
-      <c r="D6" s="9">
-        <f t="shared" si="0"/>
+      <c r="D6" s="8">
+        <f t="shared" si="2"/>
         <v>-5.9264707878838863E-3</v>
       </c>
-      <c r="N6" s="19">
+      <c r="N6" s="13">
         <v>0.5</v>
       </c>
       <c r="O6" s="3">
         <v>10</v>
       </c>
-      <c r="P6" s="9">
-        <f>N6*T$21+U$21</f>
+      <c r="P6" s="8">
+        <f t="shared" si="1"/>
         <v>9.3563811489508151</v>
       </c>
-      <c r="Q6" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q6" s="8">
+        <f t="shared" si="3"/>
         <v>0.64361885104918493</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC6" s="19">
+        <v>79</v>
+      </c>
+      <c r="AC6" s="13">
         <f>_xlfn.STDEV.P(AC3:AL3)/SQRT(COUNTA(AC3:AL3))</f>
-        <v>0.6008327554319921</v>
+        <v>0.42895221179054438</v>
       </c>
     </row>
     <row r="7" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
@@ -10623,34 +11922,34 @@
       <c r="B7" s="3">
         <v>11</v>
       </c>
-      <c r="C7" s="9">
-        <f>A7*G$21+H$21</f>
+      <c r="C7" s="8">
+        <f t="shared" si="0"/>
         <v>11.087135905255455</v>
       </c>
-      <c r="D7" s="9">
-        <f t="shared" si="0"/>
+      <c r="D7" s="8">
+        <f t="shared" si="2"/>
         <v>-8.713590525545456E-2</v>
       </c>
-      <c r="N7" s="19">
+      <c r="N7" s="13">
         <v>0.6</v>
       </c>
       <c r="O7" s="3">
         <v>12</v>
       </c>
-      <c r="P7" s="9">
-        <f>N7*T$21+U$21</f>
+      <c r="P7" s="8">
+        <f t="shared" si="1"/>
         <v>11.669074647402827</v>
       </c>
-      <c r="Q7" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q7" s="8">
+        <f t="shared" si="3"/>
         <v>0.33092535259717337</v>
       </c>
       <c r="AB7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AC7" s="8">
+      <c r="AC7" s="37">
         <f>1 + ($L$20*AC5)/(2*$L$22)</f>
-        <v>1.0002140973333333</v>
+        <v>1.0002172613333333</v>
       </c>
     </row>
     <row r="8" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
@@ -10660,34 +11959,34 @@
       <c r="B8" s="3">
         <v>14</v>
       </c>
-      <c r="C8" s="9">
-        <f>A8*G$21+H$21</f>
+      <c r="C8" s="8">
+        <f t="shared" si="0"/>
         <v>14.168345339723029</v>
       </c>
-      <c r="D8" s="9">
-        <f t="shared" si="0"/>
+      <c r="D8" s="8">
+        <f t="shared" si="2"/>
         <v>-0.16834533972302879</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="13">
         <v>0.7</v>
       </c>
       <c r="O8" s="3">
         <v>14</v>
       </c>
-      <c r="P8" s="9">
-        <f>N8*T$21+U$21</f>
+      <c r="P8" s="8">
+        <f t="shared" si="1"/>
         <v>13.981768145854836</v>
       </c>
-      <c r="Q8" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q8" s="8">
+        <f t="shared" si="3"/>
         <v>1.8231854145163595E-2</v>
       </c>
       <c r="AB8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AC8" s="8">
+      <c r="AC8" s="37">
         <f>SQRT((L20*2/((2*L22)^2)*L22*AC6)^2 + (L20*2/((2*L22)^2)*AC5*L23)^2)</f>
-        <v>9.5438754474295912E-6</v>
+        <v>8.5389653030340718E-6</v>
       </c>
     </row>
     <row r="9" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
@@ -10697,34 +11996,34 @@
       <c r="B9" s="3">
         <v>18</v>
       </c>
-      <c r="C9" s="9">
-        <f>A9*G$21+H$21</f>
+      <c r="C9" s="8">
+        <f t="shared" si="0"/>
         <v>17.249554774190603</v>
       </c>
-      <c r="D9" s="9">
-        <f t="shared" si="0"/>
+      <c r="D9" s="8">
+        <f t="shared" si="2"/>
         <v>0.75044522580939699</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="13">
         <v>0.8</v>
       </c>
       <c r="O9" s="3">
         <v>16</v>
       </c>
-      <c r="P9" s="9">
-        <f>N9*T$21+U$21</f>
+      <c r="P9" s="8">
+        <f t="shared" si="1"/>
         <v>16.29446164430685</v>
       </c>
-      <c r="Q9" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q9" s="8">
+        <f t="shared" si="3"/>
         <v>-0.29446164430684973</v>
       </c>
       <c r="AB9" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AC9" s="23">
+      <c r="AC9" s="38">
         <f>AC8/AC7</f>
-        <v>9.5418325665219862E-6</v>
+        <v>8.5371105190198948E-6</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
@@ -10734,34 +12033,34 @@
       <c r="B10" s="3">
         <v>20</v>
       </c>
-      <c r="C10" s="9">
-        <f>A10*G$21+H$21</f>
+      <c r="C10" s="8">
+        <f t="shared" si="0"/>
         <v>20.330764208658177</v>
       </c>
-      <c r="D10" s="9">
-        <f t="shared" si="0"/>
+      <c r="D10" s="8">
+        <f t="shared" si="2"/>
         <v>-0.33076420865817724</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="13">
         <v>0.9</v>
       </c>
       <c r="O10" s="3">
         <v>18</v>
       </c>
-      <c r="P10" s="9">
-        <f>N10*T$21+U$21</f>
+      <c r="P10" s="8">
+        <f t="shared" si="1"/>
         <v>18.607155142758863</v>
       </c>
-      <c r="Q10" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q10" s="8">
+        <f t="shared" si="3"/>
         <v>-0.60715514275886306</v>
       </c>
       <c r="AB10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AC10" s="12">
+      <c r="AC10" s="11">
         <f>ABS(AC7-L21)/L21</f>
-        <v>7.5880661274802181E-5</v>
+        <v>7.2717578568786971E-5</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.3">
@@ -10771,26 +12070,26 @@
       <c r="B11" s="3">
         <v>22</v>
       </c>
-      <c r="C11" s="9">
-        <f>A11*G$21+H$21</f>
+      <c r="C11" s="8">
+        <f t="shared" si="0"/>
         <v>23.411973643125748</v>
       </c>
-      <c r="D11" s="9">
-        <f t="shared" si="0"/>
+      <c r="D11" s="8">
+        <f t="shared" si="2"/>
         <v>-1.4119736431257479</v>
       </c>
-      <c r="N11" s="19">
+      <c r="N11" s="13">
         <v>1</v>
       </c>
       <c r="O11" s="3">
         <v>21</v>
       </c>
-      <c r="P11" s="9">
-        <f>N11*T$21+U$21</f>
+      <c r="P11" s="8">
+        <f t="shared" si="1"/>
         <v>20.919848641210873</v>
       </c>
-      <c r="Q11" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q11" s="8">
+        <f t="shared" si="3"/>
         <v>8.0151358789127158E-2</v>
       </c>
     </row>
@@ -10801,26 +12100,26 @@
       <c r="B12" s="3">
         <v>28</v>
       </c>
-      <c r="C12" s="9">
-        <f>A12*G$21+H$21</f>
+      <c r="C12" s="8">
+        <f t="shared" si="0"/>
         <v>26.493183077593322</v>
       </c>
-      <c r="D12" s="9">
-        <f t="shared" si="0"/>
+      <c r="D12" s="8">
+        <f t="shared" si="2"/>
         <v>1.5068169224066779</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N12" s="13">
         <v>1.1000000000000001</v>
       </c>
       <c r="O12" s="3">
         <v>22</v>
       </c>
-      <c r="P12" s="9">
-        <f>N12*T$21+U$21</f>
+      <c r="P12" s="8">
+        <f t="shared" si="1"/>
         <v>23.232542139662886</v>
       </c>
-      <c r="Q12" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q12" s="8">
+        <f t="shared" si="3"/>
         <v>-1.2325421396628862</v>
       </c>
     </row>
@@ -10831,26 +12130,26 @@
       <c r="B13" s="3">
         <v>32</v>
       </c>
-      <c r="C13" s="9">
-        <f>A13*G$21+H$21</f>
+      <c r="C13" s="8">
+        <f t="shared" si="0"/>
         <v>32.655601946528471</v>
       </c>
-      <c r="D13" s="9">
-        <f t="shared" si="0"/>
+      <c r="D13" s="8">
+        <f t="shared" si="2"/>
         <v>-0.65560194652847059</v>
       </c>
-      <c r="N13" s="19">
+      <c r="N13" s="13">
         <v>1.2</v>
       </c>
       <c r="O13" s="3">
         <v>24</v>
       </c>
-      <c r="P13" s="9">
-        <f>N13*T$21+U$21</f>
+      <c r="P13" s="8">
+        <f t="shared" si="1"/>
         <v>25.545235638114896</v>
       </c>
-      <c r="Q13" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q13" s="8">
+        <f t="shared" si="3"/>
         <v>-1.5452356381148959</v>
       </c>
     </row>
@@ -10861,26 +12160,26 @@
       <c r="B14" s="3">
         <v>37</v>
       </c>
-      <c r="C14" s="9">
-        <f>A14*G$21+H$21</f>
+      <c r="C14" s="8">
+        <f t="shared" si="0"/>
         <v>38.818020815463612</v>
       </c>
-      <c r="D14" s="9">
-        <f t="shared" si="0"/>
+      <c r="D14" s="8">
+        <f t="shared" si="2"/>
         <v>-1.8180208154636119</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="13">
         <v>1.3</v>
       </c>
       <c r="O14" s="3">
         <v>27</v>
       </c>
-      <c r="P14" s="9">
-        <f>N14*T$21+U$21</f>
+      <c r="P14" s="8">
+        <f t="shared" si="1"/>
         <v>27.857929136566909</v>
       </c>
-      <c r="Q14" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q14" s="8">
+        <f t="shared" si="3"/>
         <v>-0.85792913656690928</v>
       </c>
     </row>
@@ -10891,26 +12190,26 @@
       <c r="B15" s="3">
         <v>43</v>
       </c>
-      <c r="C15" s="9">
-        <f>A15*G$21+H$21</f>
+      <c r="C15" s="8">
+        <f t="shared" si="0"/>
         <v>44.980439684398753</v>
       </c>
-      <c r="D15" s="9">
-        <f t="shared" si="0"/>
+      <c r="D15" s="8">
+        <f t="shared" si="2"/>
         <v>-1.9804396843987533</v>
       </c>
-      <c r="N15" s="19">
+      <c r="N15" s="13">
         <v>1.4</v>
       </c>
       <c r="O15" s="3">
         <v>30</v>
       </c>
-      <c r="P15" s="9">
-        <f>N15*T$21+U$21</f>
+      <c r="P15" s="8">
+        <f t="shared" si="1"/>
         <v>30.170622635018916</v>
       </c>
-      <c r="Q15" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q15" s="8">
+        <f t="shared" si="3"/>
         <v>-0.1706226350189155</v>
       </c>
     </row>
@@ -10921,26 +12220,26 @@
       <c r="B16" s="3">
         <v>46</v>
       </c>
-      <c r="C16" s="9">
-        <f>A16*G$21+H$21</f>
+      <c r="C16" s="8">
+        <f t="shared" si="0"/>
         <v>48.061649118866335</v>
       </c>
-      <c r="D16" s="9">
-        <f t="shared" si="0"/>
+      <c r="D16" s="8">
+        <f t="shared" si="2"/>
         <v>-2.0616491188663346</v>
       </c>
-      <c r="N16" s="19">
+      <c r="N16" s="13">
         <v>1.5</v>
       </c>
       <c r="O16" s="3">
         <v>33</v>
       </c>
-      <c r="P16" s="9">
-        <f>N16*T$21+U$21</f>
+      <c r="P16" s="8">
+        <f t="shared" si="1"/>
         <v>32.483316133470929</v>
       </c>
-      <c r="Q16" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q16" s="8">
+        <f t="shared" si="3"/>
         <v>0.51668386652907117</v>
       </c>
     </row>
@@ -10951,26 +12250,26 @@
       <c r="B17" s="3">
         <v>49</v>
       </c>
-      <c r="C17" s="9">
-        <f>A17*G$21+H$21</f>
+      <c r="C17" s="8">
+        <f t="shared" si="0"/>
         <v>49.602253836100118</v>
       </c>
-      <c r="D17" s="9">
-        <f t="shared" si="0"/>
+      <c r="D17" s="8">
+        <f t="shared" si="2"/>
         <v>-0.60225383610011818</v>
       </c>
-      <c r="N17" s="19">
+      <c r="N17" s="13">
         <v>1.6</v>
       </c>
       <c r="O17" s="3">
         <v>35</v>
       </c>
-      <c r="P17" s="9">
-        <f>N17*T$21+U$21</f>
+      <c r="P17" s="8">
+        <f t="shared" si="1"/>
         <v>34.796009631922942</v>
       </c>
-      <c r="Q17" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q17" s="8">
+        <f t="shared" si="3"/>
         <v>0.20399036807705784</v>
       </c>
     </row>
@@ -10981,26 +12280,26 @@
       <c r="B18" s="3">
         <v>54</v>
       </c>
-      <c r="C18" s="9">
-        <f>A18*G$21+H$21</f>
+      <c r="C18" s="8">
+        <f t="shared" si="0"/>
         <v>51.759100440227414</v>
       </c>
-      <c r="D18" s="9">
-        <f t="shared" si="0"/>
+      <c r="D18" s="8">
+        <f t="shared" si="2"/>
         <v>2.2408995597725863</v>
       </c>
-      <c r="N18" s="19">
+      <c r="N18" s="13">
         <v>1.7</v>
       </c>
       <c r="O18" s="3">
         <v>38</v>
       </c>
-      <c r="P18" s="9">
-        <f>N18*T$21+U$21</f>
+      <c r="P18" s="8">
+        <f t="shared" si="1"/>
         <v>37.108703130374955</v>
       </c>
-      <c r="Q18" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q18" s="8">
+        <f t="shared" si="3"/>
         <v>0.89129686962504451</v>
       </c>
     </row>
@@ -11011,72 +12310,72 @@
       <c r="B19" s="3">
         <v>57</v>
       </c>
-      <c r="C19" s="9">
-        <f>A19*G$21+H$21</f>
+      <c r="C19" s="8">
+        <f t="shared" si="0"/>
         <v>53.607826100907964</v>
       </c>
-      <c r="D19" s="9">
-        <f t="shared" si="0"/>
+      <c r="D19" s="8">
+        <f t="shared" si="2"/>
         <v>3.392173899092036</v>
       </c>
-      <c r="N19" s="19">
+      <c r="N19" s="13">
         <v>1.8</v>
       </c>
       <c r="O19" s="3">
         <v>39</v>
       </c>
-      <c r="P19" s="9">
-        <f>N19*T$21+U$21</f>
+      <c r="P19" s="8">
+        <f t="shared" si="1"/>
         <v>39.421396628826969</v>
       </c>
-      <c r="Q19" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q19" s="8">
+        <f t="shared" si="3"/>
         <v>-0.42139662882696882</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
       <c r="K20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L20" s="4">
         <v>6.328E-7</v>
       </c>
-      <c r="N20" s="19">
+      <c r="N20" s="13">
         <v>1.9</v>
       </c>
       <c r="O20" s="3">
         <v>42</v>
       </c>
-      <c r="P20" s="9">
-        <f>N20*T$21+U$21</f>
+      <c r="P20" s="8">
+        <f t="shared" si="1"/>
         <v>41.734090127278975</v>
       </c>
-      <c r="Q20" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q20" s="8">
+        <f t="shared" si="3"/>
         <v>0.26590987272102495</v>
       </c>
-      <c r="S20" s="14" t="s">
+      <c r="S20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="14"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="V20" s="21"/>
     </row>
     <row r="21" spans="1:22" ht="15" x14ac:dyDescent="0.3">
       <c r="F21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="13">
         <f t="array" ref="G21:H23">LINEST(B4:B19,A4:A19,1,1)</f>
         <v>30.812094344675728</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="13">
         <v>-7.4001207015499801</v>
       </c>
       <c r="I21" s="2" t="s">
@@ -11088,28 +12387,28 @@
       <c r="L21" s="3">
         <v>1.0002899999999999</v>
       </c>
-      <c r="N21" s="19">
+      <c r="N21" s="13">
         <v>2</v>
       </c>
       <c r="O21" s="3">
         <v>45</v>
       </c>
-      <c r="P21" s="9">
-        <f>N21*T$21+U$21</f>
+      <c r="P21" s="8">
+        <f t="shared" si="1"/>
         <v>44.046783625730988</v>
       </c>
-      <c r="Q21" s="9">
-        <f t="shared" si="1"/>
+      <c r="Q21" s="8">
+        <f t="shared" si="3"/>
         <v>0.95321637426901162</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T21" s="19">
+      <c r="T21" s="13">
         <f t="array" ref="T21:U23">LINEST(O4:O21,N4:N21,1,1)</f>
         <v>23.126934984520116</v>
       </c>
-      <c r="U21" s="19">
+      <c r="U21" s="13">
         <v>-2.2070863433092427</v>
       </c>
       <c r="V21" s="2" t="s">
@@ -11120,10 +12419,10 @@
       <c r="F22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="13">
         <v>0.7037635139683871</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="13">
         <v>0.89900968482193522</v>
       </c>
       <c r="I22" s="2" t="s">
@@ -11138,10 +12437,10 @@
       <c r="S22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="T22" s="19">
+      <c r="T22" s="13">
         <v>0.33892458700223815</v>
       </c>
-      <c r="U22" s="19">
+      <c r="U22" s="13">
         <v>0.42759157161415734</v>
       </c>
       <c r="V22" s="2" t="s">
@@ -11152,10 +12451,10 @@
       <c r="F23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="10">
+      <c r="G23" s="9">
         <v>0.99274932078895828</v>
       </c>
-      <c r="H23" s="19">
+      <c r="H23" s="13">
         <v>1.583724954737687</v>
       </c>
       <c r="I23" s="2" t="s">
@@ -11170,10 +12469,10 @@
       <c r="S23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="T23" s="10">
+      <c r="T23" s="9">
         <v>0.99657547634395116</v>
       </c>
-      <c r="U23" s="19">
+      <c r="U23" s="13">
         <v>0.74601913356402572</v>
       </c>
       <c r="V23" s="2" t="s">
@@ -11196,14 +12495,14 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.88671875" style="1"/>
     <col min="3" max="3" width="8.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.21875" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
     <col min="7" max="11" width="8.88671875" style="1"/>
@@ -11212,42 +12511,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
     </row>
     <row r="3" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -11267,8 +12566,8 @@
       <c r="C4" s="3">
         <v>20</v>
       </c>
-      <c r="D4" s="4">
-        <f>(G$13*G$12*G$12*(SIN(RADIANS(B4))^2))/(G$13*G$12*(SIN(RADIANS(B4))^2)-C4*G$11)</f>
+      <c r="D4" s="37">
+        <f t="shared" ref="D4:D9" si="0">(G$13*G$12*G$12*(SIN(RADIANS(B4))^2))/(G$13*G$12*(SIN(RADIANS(B4))^2)-C4*G$11)</f>
         <v>1.4348106556451403</v>
       </c>
     </row>
@@ -11280,7 +12579,7 @@
         <v>30</v>
       </c>
       <c r="D5" s="3">
-        <f>(G$13*G$12*G$12*(SIN(RADIANS(B5))^2))/(G$13*G$12*(SIN(RADIANS(B5))^2)-C5*G$11)</f>
+        <f t="shared" si="0"/>
         <v>1.4620125382545501</v>
       </c>
     </row>
@@ -11292,7 +12591,7 @@
         <v>37</v>
       </c>
       <c r="D6" s="3">
-        <f>(G$13*G$12*G$12*(SIN(RADIANS(B6))^2))/(G$13*G$12*(SIN(RADIANS(B6))^2)-C6*G$11)</f>
+        <f t="shared" si="0"/>
         <v>1.4020337168286705</v>
       </c>
     </row>
@@ -11304,7 +12603,7 @@
         <v>47</v>
       </c>
       <c r="D7" s="3">
-        <f>(G$13*G$12*G$12*(SIN(RADIANS(B7))^2))/(G$13*G$12*(SIN(RADIANS(B7))^2)-C7*G$11)</f>
+        <f t="shared" si="0"/>
         <v>1.3875637355899335</v>
       </c>
     </row>
@@ -11316,7 +12615,7 @@
         <v>58</v>
       </c>
       <c r="D8" s="3">
-        <f>(G$13*G$12*G$12*(SIN(RADIANS(B8))^2))/(G$13*G$12*(SIN(RADIANS(B8))^2)-C8*G$11)</f>
+        <f t="shared" si="0"/>
         <v>1.375176031889934</v>
       </c>
     </row>
@@ -11328,26 +12627,26 @@
         <v>65</v>
       </c>
       <c r="D9" s="3">
-        <f>(G$13*G$12*G$12*(SIN(RADIANS(B9))^2))/(G$13*G$12*(SIN(RADIANS(B9))^2)-C9*G$11)</f>
+        <f t="shared" si="0"/>
         <v>1.3300709438340121</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="10">
+      <c r="C10" s="22"/>
+      <c r="D10" s="9">
         <f>AVERAGE(D4:D9)</f>
         <v>1.3986112703403737</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="10">
+      <c r="C11" s="22"/>
+      <c r="D11" s="9">
         <f>_xlfn.STDEV.P(D4:D9)/SQRT(6)</f>
         <v>1.7248884176812387E-2</v>
       </c>
@@ -11359,10 +12658,10 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="6">
         <f>D11/D10</f>
         <v>1.2332865137440658E-2</v>
@@ -11375,10 +12674,10 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="30"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="6">
         <f>ABS(D10-G15)/G15</f>
         <v>7.8041351126978395E-2</v>
@@ -11399,130 +12698,130 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>57</v>
+      <c r="D15" s="39" t="s">
+        <v>80</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="9">
         <v>1.5169999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="3">
+      <c r="B16" s="40">
         <v>5</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="40">
         <v>19</v>
       </c>
-      <c r="D16" s="3">
-        <f>(G$13*G$12*G$12*(SIN(RADIANS(B16))^2))/(G$13*G$12*(SIN(RADIANS(B16))^2)-C16*G$11)</f>
+      <c r="D16" s="40">
+        <f t="shared" ref="D16:D21" si="1">(G$13*G$12*G$12*(SIN(RADIANS(B16))^2))/(G$13*G$12*(SIN(RADIANS(B16))^2)-C16*G$11)</f>
         <v>1.404309428324845</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="3">
+      <c r="B17" s="40">
         <v>6</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="40">
         <v>28</v>
       </c>
-      <c r="D17" s="3">
-        <f>(G$13*G$12*G$12*(SIN(RADIANS(B17))^2))/(G$13*G$12*(SIN(RADIANS(B17))^2)-C17*G$11)</f>
+      <c r="D17" s="40">
+        <f t="shared" si="1"/>
         <v>1.4183657663638081</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="3">
+      <c r="B18" s="40">
         <v>7</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="40">
         <v>37</v>
       </c>
-      <c r="D18" s="3">
-        <f>(G$13*G$12*G$12*(SIN(RADIANS(B18))^2))/(G$13*G$12*(SIN(RADIANS(B18))^2)-C18*G$11)</f>
+      <c r="D18" s="40">
+        <f t="shared" si="1"/>
         <v>1.4020337168286705</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="3">
+      <c r="B19" s="40">
         <v>8</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="40">
         <v>45</v>
       </c>
-      <c r="D19" s="3">
-        <f>(G$13*G$12*G$12*(SIN(RADIANS(B19))^2))/(G$13*G$12*(SIN(RADIANS(B19))^2)-C19*G$11)</f>
+      <c r="D19" s="40">
+        <f t="shared" si="1"/>
         <v>1.3650741986505885</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="3">
+      <c r="B20" s="40">
         <v>9</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="40">
         <v>58</v>
       </c>
-      <c r="D20" s="4">
-        <f>(G$13*G$12*G$12*(SIN(RADIANS(B20))^2))/(G$13*G$12*(SIN(RADIANS(B20))^2)-C20*G$11)</f>
+      <c r="D20" s="41">
+        <f t="shared" si="1"/>
         <v>1.375176031889934</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="3">
+      <c r="B21" s="40">
         <v>10</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="40">
         <v>68</v>
       </c>
-      <c r="D21" s="3">
-        <f>(G$13*G$12*G$12*(SIN(RADIANS(B21))^2))/(G$13*G$12*(SIN(RADIANS(B21))^2)-C21*G$11)</f>
+      <c r="D21" s="40">
+        <f t="shared" si="1"/>
         <v>1.3506223460212641</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="10">
+      <c r="B22" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="D22" s="43">
         <f>AVERAGE(D16:D21)</f>
         <v>1.385930248013185</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B23" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="10">
+      <c r="B23" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="43">
         <f>_xlfn.STDEV.P(D16:D21)/SQRT(6)</f>
         <v>9.7844189204701823E-3</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B24" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="6">
+      <c r="B24" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="42"/>
+      <c r="D24" s="44">
         <f>D23/D22</f>
         <v>7.0598206038844594E-3</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="6">
+      <c r="C25" s="42"/>
+      <c r="D25" s="44">
         <f>ABS(D22-G15)/G15</f>
         <v>8.640062754569211E-2</v>
       </c>
@@ -11549,7 +12848,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11565,40 +12864,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -11612,7 +12911,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>9.4999999999999998E-3</v>
       </c>
       <c r="B4" s="3">
@@ -11630,7 +12929,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="B5" s="3">
@@ -11648,7 +12947,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="B6" s="3">
@@ -11661,12 +12960,12 @@
       <c r="J6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="10">
         <v>2.34</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="B7" s="3">
@@ -11679,20 +12978,20 @@
       <c r="J7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="10">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
-        <v>2.35E-2</v>
+      <c r="A8" s="10">
+        <v>2.5499999999999998E-2</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>1.8897736677640081E-4</v>
+        <v>1.7415561251942819E-4</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>64</v>
@@ -11702,7 +13001,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>2.7E-2</v>
       </c>
       <c r="B9" s="3">
@@ -11714,7 +13013,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="B10" s="3">
@@ -11726,7 +13025,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="B11" s="3">
@@ -11738,43 +13037,43 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="30"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="4">
         <f>AVERAGE(C4:C11)</f>
-        <v>1.6825717035044488E-4</v>
+        <v>1.6640445106832331E-4</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="21">
+      <c r="B13" s="22"/>
+      <c r="C13" s="15">
         <f>_xlfn.STDEV.P(C4:C11)/SQRT(COUNTA(C4:C11))</f>
-        <v>3.2515040969337375E-6</v>
+        <v>1.9946427440772595E-6</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="30"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="6">
         <f>C13/C12</f>
-        <v>1.9324609406906862E-2</v>
+        <v>1.1986715086474985E-2</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="30"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="6">
         <f>ABS(C12-K8)/K8</f>
-        <v>5.160731469028039E-2</v>
+        <v>4.0027819177020571E-2</v>
       </c>
     </row>
   </sheetData>
@@ -11794,8 +13093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D173081-7852-47E0-A7A6-CA8790E2233F}">
   <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11807,56 +13106,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
     </row>
     <row r="2" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -11894,7 +13193,7 @@
       <c r="D10" s="4">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="28">
         <v>1.8499999999999999E-2</v>
       </c>
       <c r="L10" s="5" t="s">
@@ -11917,11 +13216,11 @@
       <c r="D11" s="4">
         <v>1.2E-2</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="29"/>
       <c r="L11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="10">
         <v>2.36</v>
       </c>
     </row>
@@ -11938,11 +13237,11 @@
       <c r="D12" s="4">
         <v>1.35E-2</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="30"/>
       <c r="L12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="10">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
@@ -11950,11 +13249,11 @@
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="14">
         <f>AVERAGE(B10:B12)</f>
         <v>4.333333333333334E-3</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="14">
         <f>AVERAGE(C10:C12)</f>
         <v>7.6666666666666662E-3</v>
       </c>
@@ -11977,19 +13276,19 @@
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="15">
         <f>_xlfn.STDEV.P(B10:B12)/SQRT(3)</f>
         <v>1.3608276348795424E-4</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="15">
         <f>_xlfn.STDEV.P(C10:C12)/SQRT(3)</f>
         <v>2.721655269759087E-4</v>
       </c>
-      <c r="D14" s="21">
-        <f t="shared" ref="D14:E14" si="1">_xlfn.STDEV.P(D10:D12)/SQRT(3)</f>
+      <c r="D14" s="15">
+        <f t="shared" ref="D14" si="1">_xlfn.STDEV.P(D10:D12)/SQRT(3)</f>
         <v>3.6004114991154771E-4</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="15">
         <f>M14</f>
         <v>5.0000000000000001E-4</v>
       </c>
@@ -12026,49 +13325,49 @@
       <c r="A16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="33">
+      <c r="B16" s="24">
         <f>AVERAGE(B15:E15)</f>
         <v>3.9466298308136718E-4</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="36">
+      <c r="B17" s="27">
         <f>_xlfn.STDEV.P(B15:E15)/SQRT(COUNTA(B15:E15))</f>
         <v>1.7932394288441141E-5</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="23">
         <f>B17/B16</f>
         <v>4.5437233936743544E-2</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="23">
         <f>ABS(B16-M13)/M13</f>
         <v>1.3342542296582105E-2</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -12100,40 +13399,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -12163,18 +13462,18 @@
         <f>ABS(B4)*K$6*K$4/(K$5*A4)</f>
         <v>6.0731187955492917E-5</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="31">
         <f>AVERAGE(C4:C11)</f>
         <v>3.8888126178535052E-5</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="31">
         <f>_xlfn.STDEV.P(C4:C11)/SQRT(COUNTA(C4:C11))</f>
         <v>3.7376974630495201E-6</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="16"/>
+      <c r="H4" s="32"/>
       <c r="J4" s="2" t="s">
         <v>19</v>
       </c>
@@ -12193,10 +13492,10 @@
         <f t="shared" ref="C5:C11" si="0">ABS(B5)*K$6*K$4/(K$5*A5)</f>
         <v>5.0609323296244094E-5</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
       <c r="J5" s="5" t="s">
         <v>51</v>
       </c>
@@ -12215,14 +13514,14 @@
         <f t="shared" si="0"/>
         <v>3.7956992472183071E-5</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
       <c r="J6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="8">
         <v>0.48</v>
       </c>
     </row>
@@ -12237,14 +13536,14 @@
         <f t="shared" si="0"/>
         <v>3.9181411584188975E-5</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
       <c r="J7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="10">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
@@ -12259,8 +13558,8 @@
         <f t="shared" si="0"/>
         <v>3.1412683425254956E-5</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
@@ -12273,8 +13572,8 @@
         <f t="shared" si="0"/>
         <v>3.253456497615692E-5</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
@@ -12287,8 +13586,8 @@
         <f t="shared" si="0"/>
         <v>2.948115920169559E-5</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
@@ -12301,8 +13600,8 @@
         <f t="shared" si="0"/>
         <v>2.9197686517063899E-5</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -12332,179 +13631,179 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="17" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17">
         <v>1</v>
       </c>
-      <c r="C4" s="26" t="e">
+      <c r="C4" s="17" t="e">
         <f>ABS(B4)*K$6*K$4/(K$5*A4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D4" s="27" t="e">
+      <c r="D4" s="34" t="e">
         <f>AVERAGE(C4:C11)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E4" s="27" t="e">
+      <c r="E4" s="34" t="e">
         <f>_xlfn.STDEV.P(C4:C11)/SQRT(COUNTA(C4:C11))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="28">
+      <c r="K4" s="18">
         <v>6.328E-7</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17">
         <v>-1</v>
       </c>
-      <c r="C5" s="26" t="e">
+      <c r="C5" s="17" t="e">
         <f t="shared" ref="C5:C11" si="0">ABS(B5)*K$6*K$4/(K$5*A5)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="J5" s="29" t="s">
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="J5" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="17">
         <v>1.0002899999999999</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17">
         <v>2</v>
       </c>
-      <c r="C6" s="26" t="e">
+      <c r="C6" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="J6" s="26" t="s">
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="J6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="28"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17">
         <v>-2</v>
       </c>
-      <c r="C7" s="26" t="e">
+      <c r="C7" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="J7" s="26" t="s">
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="J7" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="28"/>
+      <c r="K7" s="18"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17">
         <v>3</v>
       </c>
-      <c r="C8" s="26" t="e">
+      <c r="C8" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17">
         <v>-3</v>
       </c>
-      <c r="C9" s="26" t="e">
+      <c r="C9" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17">
         <v>4</v>
       </c>
-      <c r="C10" s="26" t="e">
+      <c r="C10" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17">
         <v>-4</v>
       </c>
-      <c r="C11" s="26" t="e">
+      <c r="C11" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Excel T4 - (quase) acabado
</commit_message>
<xml_diff>
--- a/EXP 3/T3.xlsx
+++ b/EXP 3/T3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAIII\EXP 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8D89A3-970F-44FF-99C3-36625C0D0F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D27FB80-5763-4873-A460-83656B977CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{CAF38A1F-BD9D-416B-BE17-8DE3D13292B8}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="86">
   <si>
     <t>Determinação do n do ar - Método 1</t>
   </si>
@@ -609,6 +609,12 @@
       <t xml:space="preserve"> médio) (%)</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
 </sst>
 </file>
 
@@ -623,8 +629,8 @@
     <numFmt numFmtId="169" formatCode="0.0E+00"/>
     <numFmt numFmtId="170" formatCode="0E+00"/>
     <numFmt numFmtId="171" formatCode="0.000E+00"/>
-    <numFmt numFmtId="174" formatCode="0.000000"/>
-    <numFmt numFmtId="175" formatCode="0.00000%"/>
+    <numFmt numFmtId="172" formatCode="0.000000"/>
+    <numFmt numFmtId="173" formatCode="0.00000%"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -713,7 +719,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -819,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -869,13 +875,43 @@
     <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -885,6 +921,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -917,40 +956,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3701,7 +3713,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3714,15 +3726,15 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1600"/>
               <a:t>Y</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="-25000"/>
+              <a:rPr lang="en-US" sz="1600" baseline="-25000"/>
               <a:t>min</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1600"/>
               <a:t>(m)</a:t>
             </a:r>
           </a:p>
@@ -3741,7 +3753,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3759,7 +3771,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17742592571492333"/>
+          <c:y val="0.18495830154759849"/>
+          <c:w val="0.79723694204444873"/>
+          <c:h val="0.64944050518926455"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -3893,6 +3915,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>m (s.u.)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3955,6 +4032,77 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Y</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="-25000"/>
+                  <a:t>min </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t>(m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.7896757463646776E-2"/>
+              <c:y val="0.3762875243850336"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3993,7 +4141,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="969635536"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="-222"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -4532,12 +4680,6 @@
                 <c:pt idx="5">
                   <c:v>-3</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-4</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4547,6 +4689,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4972,12 +5132,6 @@
                 <c:pt idx="5">
                   <c:v>-3</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-4</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4987,6 +5141,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -10568,15 +10740,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>289892</xdr:colOff>
+      <xdr:colOff>256761</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>38929</xdr:rowOff>
+      <xdr:rowOff>52181</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>144118</xdr:colOff>
+      <xdr:colOff>110987</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>38929</xdr:rowOff>
+      <xdr:rowOff>52181</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11209,7 +11381,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11225,40 +11397,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
@@ -11397,7 +11569,7 @@
         <f>B4</f>
         <v>12</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="17">
         <f>B7</f>
         <v>12</v>
       </c>
@@ -11414,7 +11586,7 @@
         <f>C4</f>
         <v>10.5</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="17">
         <f>C7+B8</f>
         <v>22.5</v>
       </c>
@@ -11436,7 +11608,7 @@
       <c r="B9" s="13">
         <v>11.5</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="17">
         <f>C8+B9</f>
         <v>34</v>
       </c>
@@ -11466,7 +11638,7 @@
       <c r="B10" s="13">
         <v>10.7</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="17">
         <f t="shared" ref="C10:C16" si="2">C9+B10</f>
         <v>44.7</v>
       </c>
@@ -11495,7 +11667,7 @@
       <c r="B11" s="13">
         <v>11.3</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="17">
         <f t="shared" si="2"/>
         <v>56</v>
       </c>
@@ -11524,7 +11696,7 @@
       <c r="B12" s="13">
         <v>10</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="17">
         <f t="shared" si="2"/>
         <v>66</v>
       </c>
@@ -11553,7 +11725,7 @@
       <c r="B13" s="13">
         <v>11.1</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="17">
         <f t="shared" si="2"/>
         <v>77.099999999999994</v>
       </c>
@@ -11582,7 +11754,7 @@
       <c r="B14" s="13">
         <v>11</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="17">
         <f t="shared" si="2"/>
         <v>88.1</v>
       </c>
@@ -11605,7 +11777,7 @@
       <c r="B15" s="13">
         <v>12</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="17">
         <f t="shared" si="2"/>
         <v>100.1</v>
       </c>
@@ -11621,7 +11793,7 @@
       <c r="B16" s="13">
         <v>11</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="17">
         <f t="shared" si="2"/>
         <v>111.1</v>
       </c>
@@ -11635,7 +11807,7 @@
       <c r="G16" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H16" s="36">
+      <c r="H16" s="18">
         <f>N5/(2*G9)</f>
         <v>0.86395631067961154</v>
       </c>
@@ -11652,10 +11824,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A1DA6F-08FA-487A-82B4-E9BF2212A846}">
-  <dimension ref="A1:AM23"/>
+  <dimension ref="A1:AM26"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AK12" sqref="AK12"/>
+    <sheetView topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD18" sqref="AD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11669,88 +11841,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="20"/>
-      <c r="AJ1" s="20"/>
-      <c r="AK1" s="20"/>
-      <c r="AL1" s="20"/>
-      <c r="AM1" s="20"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
     </row>
     <row r="2" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="30"/>
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30"/>
+      <c r="AE2" s="30"/>
+      <c r="AF2" s="30"/>
+      <c r="AG2" s="30"/>
+      <c r="AH2" s="30"/>
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="30"/>
+      <c r="AK2" s="30"/>
+      <c r="AL2" s="30"/>
+      <c r="AM2" s="30"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -11947,7 +12119,7 @@
       <c r="AB7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AC7" s="37">
+      <c r="AC7" s="19">
         <f>1 + ($L$20*AC5)/(2*$L$22)</f>
         <v>1.0002172613333333</v>
       </c>
@@ -11984,7 +12156,7 @@
       <c r="AB8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AC8" s="37">
+      <c r="AC8" s="19">
         <f>SQRT((L20*2/((2*L22)^2)*L22*AC6)^2 + (L20*2/((2*L22)^2)*AC5*L23)^2)</f>
         <v>8.5389653030340718E-6</v>
       </c>
@@ -12021,7 +12193,7 @@
       <c r="AB9" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AC9" s="38">
+      <c r="AC9" s="20">
         <f>AC8/AC7</f>
         <v>8.5371105190198948E-6</v>
       </c>
@@ -12243,7 +12415,7 @@
         <v>0.51668386652907117</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>1.85</v>
       </c>
@@ -12273,7 +12445,7 @@
         <v>0.20399036807705784</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>1.92</v>
       </c>
@@ -12303,7 +12475,7 @@
         <v>0.89129686962504451</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>1.98</v>
       </c>
@@ -12333,13 +12505,13 @@
         <v>-0.42139662882696882</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="F20" s="21" t="s">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="F20" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
       <c r="K20" s="2" t="s">
         <v>19</v>
       </c>
@@ -12360,14 +12532,14 @@
         <f t="shared" si="3"/>
         <v>0.26590987272102495</v>
       </c>
-      <c r="S20" s="21" t="s">
+      <c r="S20" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="31"/>
+      <c r="V20" s="31"/>
     </row>
-    <row r="21" spans="1:22" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" ht="15" x14ac:dyDescent="0.3">
       <c r="F21" s="2" t="s">
         <v>26</v>
       </c>
@@ -12415,7 +12587,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F22" s="2" t="s">
         <v>27</v>
       </c>
@@ -12447,7 +12619,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F23" s="2" t="s">
         <v>28</v>
       </c>
@@ -12477,6 +12649,11 @@
       </c>
       <c r="V23" s="2" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA26" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -12495,7 +12672,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="B3" sqref="B3:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12511,42 +12688,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
     </row>
     <row r="3" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -12566,7 +12743,7 @@
       <c r="C4" s="3">
         <v>20</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="19">
         <f t="shared" ref="D4:D9" si="0">(G$13*G$12*G$12*(SIN(RADIANS(B4))^2))/(G$13*G$12*(SIN(RADIANS(B4))^2)-C4*G$11)</f>
         <v>1.4348106556451403</v>
       </c>
@@ -12632,20 +12809,20 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="9">
         <f>AVERAGE(D4:D9)</f>
         <v>1.3986112703403737</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="22"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="9">
         <f>_xlfn.STDEV.P(D4:D9)/SQRT(6)</f>
         <v>1.7248884176812387E-2</v>
@@ -12658,10 +12835,10 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="6">
         <f>D11/D10</f>
         <v>1.2332865137440658E-2</v>
@@ -12674,10 +12851,10 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="6">
         <f>ABS(D10-G15)/G15</f>
         <v>7.8041351126978395E-2</v>
@@ -12698,13 +12875,13 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="21" t="s">
         <v>80</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -12715,113 +12892,113 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="40">
+      <c r="B16" s="22">
         <v>5</v>
       </c>
-      <c r="C16" s="40">
+      <c r="C16" s="22">
         <v>19</v>
       </c>
-      <c r="D16" s="40">
+      <c r="D16" s="22">
         <f t="shared" ref="D16:D21" si="1">(G$13*G$12*G$12*(SIN(RADIANS(B16))^2))/(G$13*G$12*(SIN(RADIANS(B16))^2)-C16*G$11)</f>
         <v>1.404309428324845</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="40">
+      <c r="B17" s="22">
         <v>6</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="22">
         <v>28</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="22">
         <f t="shared" si="1"/>
         <v>1.4183657663638081</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="40">
+      <c r="B18" s="22">
         <v>7</v>
       </c>
-      <c r="C18" s="40">
+      <c r="C18" s="22">
         <v>37</v>
       </c>
-      <c r="D18" s="40">
+      <c r="D18" s="22">
         <f t="shared" si="1"/>
         <v>1.4020337168286705</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="40">
+      <c r="B19" s="22">
         <v>8</v>
       </c>
-      <c r="C19" s="40">
+      <c r="C19" s="22">
         <v>45</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="22">
         <f t="shared" si="1"/>
         <v>1.3650741986505885</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="40">
+      <c r="B20" s="22">
         <v>9</v>
       </c>
-      <c r="C20" s="40">
+      <c r="C20" s="22">
         <v>58</v>
       </c>
-      <c r="D20" s="41">
+      <c r="D20" s="23">
         <f t="shared" si="1"/>
         <v>1.375176031889934</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="40">
+      <c r="B21" s="22">
         <v>10</v>
       </c>
-      <c r="C21" s="40">
+      <c r="C21" s="22">
         <v>68</v>
       </c>
-      <c r="D21" s="40">
+      <c r="D21" s="22">
         <f t="shared" si="1"/>
         <v>1.3506223460212641</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="43">
+      <c r="C22" s="33"/>
+      <c r="D22" s="24">
         <f>AVERAGE(D16:D21)</f>
         <v>1.385930248013185</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="43">
+      <c r="C23" s="33"/>
+      <c r="D23" s="24">
         <f>_xlfn.STDEV.P(D16:D21)/SQRT(6)</f>
         <v>9.7844189204701823E-3</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="44">
+      <c r="C24" s="33"/>
+      <c r="D24" s="25">
         <f>D23/D22</f>
         <v>7.0598206038844594E-3</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="42"/>
-      <c r="D25" s="44">
+      <c r="C25" s="33"/>
+      <c r="D25" s="25">
         <f>ABS(D22-G15)/G15</f>
         <v>8.640062754569211E-2</v>
       </c>
@@ -12848,7 +13025,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="A3" sqref="A3:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12864,40 +13041,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
     </row>
     <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -13037,40 +13214,40 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="22"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="4">
         <f>AVERAGE(C4:C11)</f>
         <v>1.6640445106832331E-4</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="22"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="15">
         <f>_xlfn.STDEV.P(C4:C11)/SQRT(COUNTA(C4:C11))</f>
         <v>1.9946427440772595E-6</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="22"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="6">
         <f>C13/C12</f>
         <v>1.1986715086474985E-2</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="22"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="6">
         <f>ABS(C12-K8)/K8</f>
         <v>4.0027819177020571E-2</v>
@@ -13094,7 +13271,7 @@
   <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13106,56 +13283,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
     </row>
     <row r="2" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -13193,7 +13370,7 @@
       <c r="D10" s="4">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="39">
         <v>1.8499999999999999E-2</v>
       </c>
       <c r="L10" s="5" t="s">
@@ -13216,7 +13393,7 @@
       <c r="D11" s="4">
         <v>1.2E-2</v>
       </c>
-      <c r="E11" s="29"/>
+      <c r="E11" s="40"/>
       <c r="L11" s="2" t="s">
         <v>62</v>
       </c>
@@ -13237,7 +13414,7 @@
       <c r="D12" s="4">
         <v>1.35E-2</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="L12" s="2" t="s">
         <v>63</v>
       </c>
@@ -13325,49 +13502,49 @@
       <c r="A16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="35">
         <f>AVERAGE(B15:E15)</f>
         <v>3.9466298308136718E-4</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="37"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="38">
         <f>_xlfn.STDEV.P(B15:E15)/SQRT(COUNTA(B15:E15))</f>
         <v>1.7932394288441141E-5</v>
       </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="34">
         <f>B17/B16</f>
         <v>4.5437233936743544E-2</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="23">
+      <c r="B19" s="34">
         <f>ABS(B16-M13)/M13</f>
         <v>1.3342542296582105E-2</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -13385,10 +13562,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B4B3CB5-D16A-4426-8E5D-ED09DF9E09D0}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13399,40 +13576,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -13462,18 +13639,18 @@
         <f>ABS(B4)*K$6*K$4/(K$5*A4)</f>
         <v>6.0731187955492917E-5</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="42">
         <f>AVERAGE(C4:C11)</f>
         <v>3.8888126178535052E-5</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="42">
         <f>_xlfn.STDEV.P(C4:C11)/SQRT(COUNTA(C4:C11))</f>
         <v>3.7376974630495201E-6</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="32"/>
+      <c r="H4" s="43"/>
       <c r="J4" s="2" t="s">
         <v>19</v>
       </c>
@@ -13492,10 +13669,10 @@
         <f t="shared" ref="C5:C11" si="0">ABS(B5)*K$6*K$4/(K$5*A5)</f>
         <v>5.0609323296244094E-5</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
       <c r="J5" s="5" t="s">
         <v>51</v>
       </c>
@@ -13514,10 +13691,10 @@
         <f t="shared" si="0"/>
         <v>3.7956992472183071E-5</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
       <c r="J6" s="2" t="s">
         <v>38</v>
       </c>
@@ -13536,10 +13713,10 @@
         <f t="shared" si="0"/>
         <v>3.9181411584188975E-5</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
       <c r="J7" s="2" t="s">
         <v>39</v>
       </c>
@@ -13558,8 +13735,8 @@
         <f t="shared" si="0"/>
         <v>3.1412683425254956E-5</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
@@ -13572,8 +13749,8 @@
         <f t="shared" si="0"/>
         <v>3.253456497615692E-5</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
@@ -13586,8 +13763,8 @@
         <f t="shared" si="0"/>
         <v>2.948115920169559E-5</v>
       </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
@@ -13600,8 +13777,13 @@
         <f t="shared" si="0"/>
         <v>2.9197686517063899E-5</v>
       </c>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+    </row>
+    <row r="22" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L22" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -13617,10 +13799,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74051A4E-52A8-4341-9391-645898D5A5C1}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13631,185 +13813,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="26" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17">
+      <c r="A4" s="27">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B4" s="27">
         <v>1</v>
       </c>
-      <c r="C4" s="17" t="e">
+      <c r="C4" s="28">
         <f>ABS(B4)*K$6*K$4/(K$5*A4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D4" s="34" t="e">
+        <v>5.9491259534734934E-5</v>
+      </c>
+      <c r="D4" s="44">
         <f>AVERAGE(C4:C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E4" s="34" t="e">
+        <v>6.3111098077853726E-5</v>
+      </c>
+      <c r="E4" s="44">
         <f>_xlfn.STDEV.P(C4:C11)/SQRT(COUNTA(C4:C11))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J4" s="17" t="s">
+        <v>1.1165783691493025E-6</v>
+      </c>
+      <c r="J4" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="28">
         <v>6.328E-7</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17">
+      <c r="A5" s="27">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B5" s="27">
         <v>-1</v>
       </c>
-      <c r="C5" s="17" t="e">
-        <f t="shared" ref="C5:C11" si="0">ABS(B5)*K$6*K$4/(K$5*A5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="J5" s="19" t="s">
+      <c r="C5" s="27">
+        <f t="shared" ref="C5:C9" si="0">ABS(B5)*K$6*K$4/(K$5*A5)</f>
+        <v>5.9491259534734934E-5</v>
+      </c>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="J5" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5" s="27">
         <v>1.0002899999999999</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17">
+      <c r="A6" s="27">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="B6" s="27">
         <v>2</v>
       </c>
-      <c r="C6" s="17" t="e">
+      <c r="C6" s="27">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="J6" s="17" t="s">
+        <v>6.6101399483038822E-5</v>
+      </c>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="J6" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="18"/>
+      <c r="K6" s="28">
+        <v>2.351</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17">
+      <c r="A7" s="27">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="B7" s="27">
         <v>-2</v>
       </c>
-      <c r="C7" s="17" t="e">
+      <c r="C7" s="27">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="J7" s="17" t="s">
+        <v>6.6101399483038822E-5</v>
+      </c>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="J7" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="18"/>
+      <c r="K7" s="28">
+        <v>5.0000000000000001E-4</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17">
+      <c r="A8" s="27">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B8" s="27">
         <v>3</v>
       </c>
-      <c r="C8" s="17" t="e">
+      <c r="C8" s="27">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
+        <v>6.3740635215787423E-5</v>
+      </c>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17">
+      <c r="A9" s="27">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B9" s="27">
         <v>-3</v>
       </c>
-      <c r="C9" s="17" t="e">
+      <c r="C9" s="27">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17">
-        <v>4</v>
-      </c>
-      <c r="C10" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17">
-        <v>-4</v>
-      </c>
-      <c r="C11" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
+        <v>6.3740635215787423E-5</v>
+      </c>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:O2"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="E4:E9"/>
+    <mergeCell ref="D4:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
T4 - excel versão 0 e documentos txt
</commit_message>
<xml_diff>
--- a/EXP 3/T3.xlsx
+++ b/EXP 3/T3.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAIII\EXP 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D27FB80-5763-4873-A460-83656B977CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F7C4E2-461C-4E75-9A0B-062E565DECDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{CAF38A1F-BD9D-416B-BE17-8DE3D13292B8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CAF38A1F-BD9D-416B-BE17-8DE3D13292B8}"/>
   </bookViews>
   <sheets>
     <sheet name="P1.1" sheetId="1" r:id="rId1"/>
     <sheet name="P1.2" sheetId="2" r:id="rId2"/>
     <sheet name="P1.3" sheetId="3" r:id="rId3"/>
     <sheet name="P2.1" sheetId="4" r:id="rId4"/>
-    <sheet name="P2.3" sheetId="7" r:id="rId5"/>
-    <sheet name="P2.1 FENDA MULTIPLA" sheetId="8" r:id="rId6"/>
-    <sheet name="P2.2" sheetId="5" r:id="rId7"/>
+    <sheet name="P2.2" sheetId="5" r:id="rId5"/>
+    <sheet name="P2.3" sheetId="7" r:id="rId6"/>
+    <sheet name="P2.1 FENDA MULTIPLA" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="86">
   <si>
     <t>Determinação do n do ar - Método 1</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t>u(m)</t>
-  </si>
-  <si>
-    <t>r^2</t>
   </si>
   <si>
     <t>b</t>
@@ -615,6 +612,22 @@
   <si>
     <t>\</t>
   </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -632,7 +645,7 @@
     <numFmt numFmtId="172" formatCode="0.000000"/>
     <numFmt numFmtId="173" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -687,6 +700,14 @@
       <vertAlign val="subscript"/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2349,7 +2370,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Resíduos</a:t>
+                  <a:t>N - N</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="-25000"/>
+                  <a:t>ajuste</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400" baseline="0"/>
@@ -3565,7 +3590,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Resíduos (s.u.)</a:t>
+                  <a:t>N-N</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="-25000"/>
+                  <a:t>ajuste</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t> (s.u.)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3735,7 +3768,11 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1600"/>
-              <a:t>(m)</a:t>
+              <a:t>(m) -</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0"/>
+              <a:t> Fenda</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3776,9 +3813,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17742592571492333"/>
+          <c:x val="0.16650474802499748"/>
           <c:y val="0.18495830154759849"/>
-          <c:w val="0.79723694204444873"/>
+          <c:w val="0.80815811973437457"/>
           <c:h val="0.64944050518926455"/>
         </c:manualLayout>
       </c:layout>
@@ -4230,9 +4267,18 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Traçado deverá ser simétrico</a:t>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>Y</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="-25000"/>
+              <a:t>min</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0"/>
+              <a:t>(m) - Fio de Cabelo</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1600"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4267,7 +4313,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12462270341207349"/>
+          <c:y val="0.15523148148148147"/>
+          <c:w val="0.85237729658792649"/>
+          <c:h val="0.68602653834937299"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -4298,7 +4354,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'P2.1 FENDA MULTIPLA'!$B$4:$B$11</c:f>
+              <c:f>'P2.2'!$C$4:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4320,44 +4376,32 @@
                 <c:pt idx="5">
                   <c:v>-3</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-5</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'P2.1 FENDA MULTIPLA'!$A$4:$A$11</c:f>
+              <c:f>'P2.2'!$B$4:$B$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6E-2</c:v>
+                  <c:v>4.4999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.55E-2</c:v>
+                  <c:v>4.4999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9000000000000001E-2</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.8000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.1499999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.1999999999999998E-2</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4365,7 +4409,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-37EB-4B14-95F9-F538CD7FC9DD}"/>
+              <c16:uniqueId val="{00000000-5ADF-4677-8CC9-209CEA30E743}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4401,6 +4445,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>m</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> (s.u.)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4463,7 +4567,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Y</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="-25000"/>
+                  <a:t>min</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t> (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4501,7 +4668,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="969635536"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="-5000"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -4557,354 +4724,6 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Traçado deverá ser simétrico</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'P2.2'!$B$4:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'P2.2'!$A$4:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2.5000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.5000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.4999999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.4999999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.0000000000000007E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.0000000000000007E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5ADF-4677-8CC9-209CEA30E743}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="969635536"/>
-        <c:axId val="1002525664"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="969635536"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1002525664"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1002525664"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="969635536"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5110,7 +4929,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'P2.2'!$B$4:$B$11</c:f>
+              <c:f>'P2.2'!$C$4:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5137,7 +4956,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'P2.2'!$A$4:$A$11</c:f>
+              <c:f>'P2.2'!$B$4:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5302,6 +5121,503 @@
         </c:txPr>
         <c:crossAx val="969635536"/>
         <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>Y</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="-25000"/>
+              <a:t>min</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>(m) - Fenda Dupla</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16349781277340336"/>
+          <c:y val="0.1413425925925926"/>
+          <c:w val="0.81350218722659662"/>
+          <c:h val="0.71843394575678043"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'P2.1 FENDA MULTIPLA'!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'P2.1 FENDA MULTIPLA'!$B$4:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.55E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.1499999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.1999999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-37EB-4B14-95F9-F538CD7FC9DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="969635536"/>
+        <c:axId val="1002525664"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="969635536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t>m (s.u.)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1002525664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1002525664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Y</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="-25000"/>
+                  <a:t>min </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t>(m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="969635536"/>
+        <c:crossesAt val="-55"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -10780,13 +11096,138 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>365761</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>97591</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85B649B2-E4D2-4A70-A446-13F0FF6D1791}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7315201" y="548640"/>
+          <a:ext cx="3413760" cy="1019611"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A46010AF-3560-45A7-8D2D-D88102486F4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76E686EB-E67D-4470-B74B-4B38FEC96FC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>158697</xdr:rowOff>
@@ -10824,13 +11265,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>238206</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>417</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>1986</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -10869,17 +11310,17 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>365761</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>97591</xdr:rowOff>
@@ -10917,14 +11358,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -10948,131 +11389,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>365761</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>97591</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85B649B2-E4D2-4A70-A446-13F0FF6D1791}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7315201" y="548640"/>
-          <a:ext cx="3413760" cy="1019611"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A46010AF-3560-45A7-8D2D-D88102486F4E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76E686EB-E67D-4470-B74B-4B38FEC96FC9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11380,8 +11696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0D8ADF-2EFB-452A-A480-0B215EA5BBF1}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11466,7 +11782,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="13">
         <v>12</v>
@@ -11507,7 +11823,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="4">
         <f>B4*10^-6</f>
@@ -11558,7 +11874,7 @@
     </row>
     <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.3">
       <c r="M6" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N6" s="3">
         <v>1.0002899999999999</v>
@@ -11627,7 +11943,7 @@
         <v>7.3333333333331502E-7</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N9" s="4">
         <f>AVERAGE(B5:K5)</f>
@@ -11656,7 +11972,7 @@
         <v>3.2487604473775323E-7</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N10" s="15">
         <f>_xlfn.STDEV.P(B5:K5)/SQRT(10)</f>
@@ -11743,7 +12059,7 @@
         <v>1.8093333333333703E-12</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N13" s="6">
         <f>N12/N11</f>
@@ -11766,7 +12082,7 @@
         <v>240</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N14" s="6">
         <f>ABS(N11-N6)/N6</f>
@@ -11805,7 +12121,7 @@
         <v>300</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H16" s="18">
         <f>N5/(2*G9)</f>
@@ -11826,8 +12142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A1DA6F-08FA-487A-82B4-E9BF2212A846}">
   <dimension ref="A1:AM26"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD18" sqref="AD18"/>
+    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11926,7 +12242,7 @@
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -11938,7 +12254,7 @@
         <v>24</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>5</v>
@@ -12043,7 +12359,7 @@
         <v>0.95631234950119648</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AC5" s="3">
         <f>AVERAGE(AC3:AL3)</f>
@@ -12080,7 +12396,7 @@
         <v>0.64361885104918493</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AC6" s="13">
         <f>_xlfn.STDEV.P(AC3:AL3)/SQRT(COUNTA(AC3:AL3))</f>
@@ -12191,7 +12507,7 @@
         <v>-0.29446164430684973</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AC9" s="20">
         <f>AC8/AC7</f>
@@ -12228,7 +12544,7 @@
         <v>-0.60715514275886306</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AC10" s="11">
         <f>ABS(AC7-L21)/L21</f>
@@ -12551,10 +12867,10 @@
         <v>-7.4001207015499801</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L21" s="3">
         <v>1.0002899999999999</v>
@@ -12584,7 +12900,7 @@
         <v>-2.2070863433092427</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.3">
@@ -12598,10 +12914,10 @@
         <v>0.89900968482193522</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L22" s="3">
         <v>0.03</v>
@@ -12616,12 +12932,12 @@
         <v>0.42759157161415734</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" ht="16.2" x14ac:dyDescent="0.3">
       <c r="F23" s="2" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="G23" s="9">
         <v>0.99274932078895828</v>
@@ -12630,16 +12946,16 @@
         <v>1.583724954737687</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L23" s="3">
         <v>1E-3</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="T23" s="9">
         <v>0.99657547634395116</v>
@@ -12648,12 +12964,12 @@
         <v>0.74601913356402572</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="AA26" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -12672,7 +12988,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D13"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12727,13 +13043,13 @@
     </row>
     <row r="3" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -12810,7 +13126,7 @@
     </row>
     <row r="10" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="9">
@@ -12820,7 +13136,7 @@
     </row>
     <row r="11" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="9">
@@ -12836,7 +13152,7 @@
     </row>
     <row r="12" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="6">
@@ -12844,7 +13160,7 @@
         <v>1.2332865137440658E-2</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G12" s="3">
         <v>1.0002899999999999</v>
@@ -12852,7 +13168,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B13" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="6">
@@ -12860,7 +13176,7 @@
         <v>7.8041351126978395E-2</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" s="4">
         <v>5.4999999999999997E-3</v>
@@ -12868,7 +13184,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14" s="4">
         <v>5.0000000000000001E-4</v>
@@ -12876,16 +13192,16 @@
     </row>
     <row r="15" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G15" s="9">
         <v>1.5169999999999999</v>
@@ -12965,7 +13281,7 @@
     </row>
     <row r="22" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" s="33"/>
       <c r="D22" s="24">
@@ -12975,7 +13291,7 @@
     </row>
     <row r="23" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C23" s="33"/>
       <c r="D23" s="24">
@@ -12985,7 +13301,7 @@
     </row>
     <row r="24" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C24" s="33"/>
       <c r="D24" s="25">
@@ -12995,7 +13311,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="33"/>
       <c r="D25" s="25">
@@ -13022,10 +13338,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C185EA-2383-490B-AEDD-2F2B95FB59CC}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C15"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13078,13 +13394,13 @@
     </row>
     <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -13117,7 +13433,7 @@
         <v>1.6448030071279331E-4</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K5" s="3">
         <v>1.0002899999999999</v>
@@ -13135,7 +13451,7 @@
         <v>1.7415561251942819E-4</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K6" s="10">
         <v>2.34</v>
@@ -13153,7 +13469,7 @@
         <v>1.6448030071279331E-4</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K7" s="10">
         <v>5.0000000000000001E-4</v>
@@ -13171,7 +13487,7 @@
         <v>1.7415561251942819E-4</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K8" s="4">
         <v>1.6000000000000001E-4</v>
@@ -13215,7 +13531,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="32"/>
       <c r="C12" s="4">
@@ -13225,7 +13541,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="32"/>
       <c r="C13" s="15">
@@ -13235,7 +13551,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="32"/>
       <c r="C14" s="6">
@@ -13245,12 +13561,22 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="6">
         <f>ABS(C12-K8)/K8</f>
         <v>4.0027819177020571E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O16" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G29" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -13267,26 +13593,222 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D173081-7852-47E0-A7A6-CA8790E2233F}">
-  <dimension ref="A1:W19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74051A4E-52A8-4341-9391-645898D5A5C1}">
+  <dimension ref="B1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" style="1" customWidth="1"/>
-    <col min="2" max="11" width="8.88671875" style="1"/>
-    <col min="12" max="12" width="16.44140625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="10" width="8.88671875" style="1"/>
+    <col min="11" max="11" width="11.88671875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="30"/>
+    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B1" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B3" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="27">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C4" s="27">
+        <v>1</v>
+      </c>
+      <c r="D4" s="28">
+        <f>ABS(C4)*L$6*L$4/(L$5*B4)</f>
+        <v>5.9491259534734934E-5</v>
+      </c>
+      <c r="E4" s="44">
+        <f>AVERAGE(D4:D11)</f>
+        <v>6.3111098077853726E-5</v>
+      </c>
+      <c r="F4" s="44">
+        <f>_xlfn.STDEV.P(D4:D11)/SQRT(COUNTA(D4:D11))</f>
+        <v>1.1165783691493025E-6</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="28">
+        <v>6.328E-7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" ht="15" x14ac:dyDescent="0.3">
+      <c r="B5" s="27">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C5" s="27">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="27">
+        <f t="shared" ref="D5:D9" si="0">ABS(C5)*L$6*L$4/(L$5*B5)</f>
+        <v>5.9491259534734934E-5</v>
+      </c>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="K5" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="27">
+        <v>1.0002899999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="27">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C6" s="27">
+        <v>2</v>
+      </c>
+      <c r="D6" s="27">
+        <f t="shared" si="0"/>
+        <v>6.6101399483038822E-5</v>
+      </c>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="K6" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="28">
+        <v>2.351</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="27">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C7" s="27">
+        <v>-2</v>
+      </c>
+      <c r="D7" s="27">
+        <f t="shared" si="0"/>
+        <v>6.6101399483038822E-5</v>
+      </c>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="K7" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="28">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="27">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C8" s="27">
+        <v>3</v>
+      </c>
+      <c r="D8" s="27">
+        <f t="shared" si="0"/>
+        <v>6.3740635215787423E-5</v>
+      </c>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="27">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C9" s="27">
+        <v>-3</v>
+      </c>
+      <c r="D9" s="27">
+        <f t="shared" si="0"/>
+        <v>6.3740635215787423E-5</v>
+      </c>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="H9" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:P2"/>
+    <mergeCell ref="F4:F9"/>
+    <mergeCell ref="E4:E9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D173081-7852-47E0-A7A6-CA8790E2233F}">
+  <dimension ref="B1:X19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="13.77734375" style="1" customWidth="1"/>
+    <col min="3" max="12" width="8.88671875" style="1"/>
+    <col min="13" max="13" width="16.44140625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="30" t="s">
+        <v>41</v>
+      </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
       <c r="E1" s="30"/>
@@ -13308,9 +13830,9 @@
       <c r="U1" s="30"/>
       <c r="V1" s="30"/>
       <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
     </row>
-    <row r="2" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
+    <row r="2" spans="2:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -13333,253 +13855,253 @@
       <c r="U2" s="30"/>
       <c r="V2" s="30"/>
       <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M9" s="4">
+      <c r="N9" s="4">
         <v>6.328E-7</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="15" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="2:24" ht="15" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="4">
+      <c r="C10" s="4">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="C10" s="4">
+      <c r="D10" s="4">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="4">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="E10" s="39">
+      <c r="F10" s="39">
         <v>1.8499999999999999E-2</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="M10" s="3">
+      <c r="M10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="N10" s="3">
         <v>1.0002899999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4">
+      <c r="C11" s="4">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="C11" s="4">
+      <c r="D11" s="4">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E11" s="4">
         <v>1.2E-2</v>
       </c>
-      <c r="E11" s="40"/>
-      <c r="L11" s="2" t="s">
+      <c r="F11" s="40"/>
+      <c r="M11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N11" s="10">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="D12" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1.35E-2</v>
+      </c>
+      <c r="F12" s="41"/>
+      <c r="M12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M11" s="10">
-        <v>2.36</v>
+      <c r="N12" s="10">
+        <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="4">
-        <v>4.4999999999999997E-3</v>
-      </c>
-      <c r="C12" s="4">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1.35E-2</v>
-      </c>
-      <c r="E12" s="41"/>
-      <c r="L12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="M12" s="10">
-        <v>5.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B13" s="14">
-        <f>AVERAGE(B10:B12)</f>
-        <v>4.333333333333334E-3</v>
       </c>
       <c r="C13" s="14">
         <f>AVERAGE(C10:C12)</f>
+        <v>4.333333333333334E-3</v>
+      </c>
+      <c r="D13" s="14">
+        <f>AVERAGE(D10:D12)</f>
         <v>7.6666666666666662E-3</v>
       </c>
-      <c r="D13" s="4">
-        <f t="shared" ref="D13" si="0">AVERAGE(D10:D12)</f>
+      <c r="E13" s="4">
+        <f t="shared" ref="E13" si="0">AVERAGE(E10:E12)</f>
         <v>1.2666666666666666E-2</v>
       </c>
-      <c r="E13" s="4">
-        <f>AVERAGE(E10)</f>
+      <c r="F13" s="4">
+        <f>AVERAGE(F10)</f>
         <v>1.8499999999999999E-2</v>
       </c>
-      <c r="L13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M13" s="4">
+      <c r="M13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N13" s="4">
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B14" s="15">
-        <f>_xlfn.STDEV.P(B10:B12)/SQRT(3)</f>
-        <v>1.3608276348795424E-4</v>
       </c>
       <c r="C14" s="15">
         <f>_xlfn.STDEV.P(C10:C12)/SQRT(3)</f>
+        <v>1.3608276348795424E-4</v>
+      </c>
+      <c r="D14" s="15">
+        <f>_xlfn.STDEV.P(D10:D12)/SQRT(3)</f>
         <v>2.721655269759087E-4</v>
       </c>
-      <c r="D14" s="15">
-        <f t="shared" ref="D14" si="1">_xlfn.STDEV.P(D10:D12)/SQRT(3)</f>
+      <c r="E14" s="15">
+        <f t="shared" ref="E14" si="1">_xlfn.STDEV.P(E10:E12)/SQRT(3)</f>
         <v>3.6004114991154771E-4</v>
       </c>
-      <c r="E14" s="15">
-        <f>M14</f>
+      <c r="F14" s="15">
+        <f>N14</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="L14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M14" s="3">
+      <c r="M14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="N14" s="3">
         <f>0.5*10^-3</f>
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="4">
-        <f>1.22*M$9*M$11/(M$10*B13)</f>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="4">
+        <f>1.22*N$9*N$11/(N$10*C13)</f>
         <v>4.2032989509965184E-4</v>
       </c>
-      <c r="C15" s="4">
-        <f>2.23*M$9*M$11/(M$10*C13)</f>
+      <c r="D15" s="4">
+        <f>2.23*N$9*N$11/(N$10*D13)</f>
         <v>4.3426099996218495E-4</v>
       </c>
-      <c r="D15" s="4">
-        <f>3.24*M$9*M$11/(M$10*D13)</f>
+      <c r="E15" s="4">
+        <f>3.24*N$9*N$11/(N$10*E13)</f>
         <v>3.8188729899907981E-4</v>
       </c>
-      <c r="E15" s="4">
-        <f>4.24*M$9*M$11/(M$10*E13)</f>
+      <c r="F15" s="4">
+        <f>4.24*N$9*N$11/(N$10*F13)</f>
         <v>3.4217373826455201E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="35">
+        <f>AVERAGE(C15:F15)</f>
+        <v>3.9466298308136718E-4</v>
+      </c>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="37"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="35">
-        <f>AVERAGE(B15:E15)</f>
-        <v>3.9466298308136718E-4</v>
-      </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="37"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="38">
-        <f>_xlfn.STDEV.P(B15:E15)/SQRT(COUNTA(B15:E15))</f>
+      <c r="C17" s="38">
+        <f>_xlfn.STDEV.P(C15:F15)/SQRT(COUNTA(C15:F15))</f>
         <v>1.7932394288441141E-5</v>
       </c>
-      <c r="C17" s="38"/>
       <c r="D17" s="38"/>
       <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="34">
-        <f>B17/B16</f>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="34">
+        <f>C17/C16</f>
         <v>4.5437233936743544E-2</v>
       </c>
-      <c r="C18" s="34"/>
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="34">
-        <f>ABS(B16-M13)/M13</f>
+      <c r="C19" s="34">
+        <f>ABS(C16-N13)/N13</f>
         <v>1.3342542296582105E-2</v>
       </c>
-      <c r="C19" s="34"/>
       <c r="D19" s="34"/>
       <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="A1:W2"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="B1:X2"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="F10:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B4B3CB5-D16A-4426-8E5D-ED09DF9E09D0}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="B1:P22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="8.88671875" style="1"/>
-    <col min="10" max="10" width="12.44140625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="10" width="8.88671875" style="1"/>
+    <col min="11" max="11" width="12.44140625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="30"/>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
       <c r="E1" s="30"/>
@@ -13593,9 +14115,9 @@
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
       <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -13610,380 +14132,191 @@
       <c r="M2" s="30"/>
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>37</v>
+      <c r="F3" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
-        <f>ABS(B4)*K$6*K$4/(K$5*A4)</f>
+      <c r="D4" s="3">
+        <f>ABS(C4)*L$6*L$4/(L$5*B4)</f>
         <v>6.0731187955492917E-5</v>
       </c>
-      <c r="D4" s="42">
-        <f>AVERAGE(C4:C11)</f>
+      <c r="E4" s="42">
+        <f>AVERAGE(D4:D11)</f>
         <v>3.8888126178535052E-5</v>
       </c>
-      <c r="E4" s="42">
-        <f>_xlfn.STDEV.P(C4:C11)/SQRT(COUNTA(C4:C11))</f>
+      <c r="F4" s="42">
+        <f>_xlfn.STDEV.P(D4:D11)/SQRT(COUNTA(D4:D11))</f>
         <v>3.7376974630495201E-6</v>
       </c>
-      <c r="G4" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="43"/>
-      <c r="J4" s="2" t="s">
+      <c r="H4" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="43"/>
+      <c r="K4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
         <v>6.328E-7</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+    <row r="5" spans="2:16" ht="15" x14ac:dyDescent="0.3">
+      <c r="B5" s="4">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="C5" s="3">
         <v>-1</v>
       </c>
-      <c r="C5" s="3">
-        <f t="shared" ref="C5:C11" si="0">ABS(B5)*K$6*K$4/(K$5*A5)</f>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D11" si="0">ABS(C5)*L$6*L$4/(L$5*B5)</f>
         <v>5.0609323296244094E-5</v>
       </c>
-      <c r="D5" s="42"/>
       <c r="E5" s="42"/>
-      <c r="G5" s="43"/>
+      <c r="F5" s="42"/>
       <c r="H5" s="43"/>
-      <c r="J5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K5" s="3">
+      <c r="I5" s="43"/>
+      <c r="K5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="3">
         <v>1.0002899999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="4">
         <v>1.6E-2</v>
       </c>
-      <c r="B6" s="3">
+      <c r="C6" s="3">
         <v>2</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="3">
         <f t="shared" si="0"/>
         <v>3.7956992472183071E-5</v>
       </c>
-      <c r="D6" s="42"/>
       <c r="E6" s="42"/>
-      <c r="G6" s="43"/>
+      <c r="F6" s="42"/>
       <c r="H6" s="43"/>
-      <c r="J6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="8">
+      <c r="I6" s="43"/>
+      <c r="K6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="8">
         <v>0.48</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
         <v>1.55E-2</v>
       </c>
-      <c r="B7" s="3">
+      <c r="C7" s="3">
         <v>-2</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <f t="shared" si="0"/>
         <v>3.9181411584188975E-5</v>
       </c>
-      <c r="D7" s="42"/>
       <c r="E7" s="42"/>
-      <c r="G7" s="43"/>
+      <c r="F7" s="42"/>
       <c r="H7" s="43"/>
-      <c r="J7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" s="10">
+      <c r="I7" s="43"/>
+      <c r="K7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="10">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="4">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="B8" s="3">
+      <c r="C8" s="3">
         <v>3</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>3.1412683425254956E-5</v>
       </c>
-      <c r="D8" s="42"/>
       <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="B9" s="3">
+      <c r="C9" s="3">
         <v>-3</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
         <v>3.253456497615692E-5</v>
       </c>
-      <c r="D9" s="42"/>
       <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="K9" s="1">
+        <v>5</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
         <v>5.1499999999999997E-2</v>
       </c>
-      <c r="B10" s="3">
+      <c r="C10" s="3">
         <v>5</v>
       </c>
-      <c r="C10" s="3">
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>2.948115920169559E-5</v>
       </c>
-      <c r="D10" s="42"/>
       <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="4">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="B11" s="3">
+      <c r="C11" s="3">
         <v>-5</v>
       </c>
-      <c r="C11" s="3">
+      <c r="D11" s="3">
         <f t="shared" si="0"/>
         <v>2.9197686517063899E-5</v>
       </c>
-      <c r="D11" s="42"/>
       <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
     </row>
-    <row r="22" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L22" s="1" t="s">
-        <v>84</v>
+    <row r="22" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M22" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:O2"/>
-    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="B1:P2"/>
     <mergeCell ref="E4:E11"/>
-    <mergeCell ref="G4:H7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74051A4E-52A8-4341-9391-645898D5A5C1}">
-  <dimension ref="A1:O9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="9" width="8.88671875" style="1"/>
-    <col min="10" max="10" width="11.88671875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="27">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="B4" s="27">
-        <v>1</v>
-      </c>
-      <c r="C4" s="28">
-        <f>ABS(B4)*K$6*K$4/(K$5*A4)</f>
-        <v>5.9491259534734934E-5</v>
-      </c>
-      <c r="D4" s="44">
-        <f>AVERAGE(C4:C11)</f>
-        <v>6.3111098077853726E-5</v>
-      </c>
-      <c r="E4" s="44">
-        <f>_xlfn.STDEV.P(C4:C11)/SQRT(COUNTA(C4:C11))</f>
-        <v>1.1165783691493025E-6</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="28">
-        <v>6.328E-7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.3">
-      <c r="A5" s="27">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="B5" s="27">
-        <v>-1</v>
-      </c>
-      <c r="C5" s="27">
-        <f t="shared" ref="C5:C9" si="0">ABS(B5)*K$6*K$4/(K$5*A5)</f>
-        <v>5.9491259534734934E-5</v>
-      </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="J5" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="K5" s="27">
-        <v>1.0002899999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="27">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="B6" s="27">
-        <v>2</v>
-      </c>
-      <c r="C6" s="27">
-        <f t="shared" si="0"/>
-        <v>6.6101399483038822E-5</v>
-      </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="J6" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="28">
-        <v>2.351</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="27">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="B7" s="27">
-        <v>-2</v>
-      </c>
-      <c r="C7" s="27">
-        <f t="shared" si="0"/>
-        <v>6.6101399483038822E-5</v>
-      </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="J7" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" s="28">
-        <v>5.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="B8" s="27">
-        <v>3</v>
-      </c>
-      <c r="C8" s="27">
-        <f t="shared" si="0"/>
-        <v>6.3740635215787423E-5</v>
-      </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="27">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="B9" s="27">
-        <v>-3</v>
-      </c>
-      <c r="C9" s="27">
-        <f t="shared" si="0"/>
-        <v>6.3740635215787423E-5</v>
-      </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:O2"/>
-    <mergeCell ref="E4:E9"/>
-    <mergeCell ref="D4:D9"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="H4:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
T7 - Excel e ficheiros
</commit_message>
<xml_diff>
--- a/EXP 3/T3.xlsx
+++ b/EXP 3/T3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAIII\EXP 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F7C4E2-461C-4E75-9A0B-062E565DECDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46994BCD-044C-4232-9B59-A99086BC8BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CAF38A1F-BD9D-416B-BE17-8DE3D13292B8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{CAF38A1F-BD9D-416B-BE17-8DE3D13292B8}"/>
   </bookViews>
   <sheets>
     <sheet name="P1.1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="87">
   <si>
     <t>Determinação do n do ar - Método 1</t>
   </si>
@@ -610,9 +610,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>\</t>
-  </si>
-  <si>
     <r>
       <t>r</t>
     </r>
@@ -628,12 +625,18 @@
       <t>2</t>
     </r>
   </si>
+  <si>
+    <t>log(p)</t>
+  </si>
+  <si>
+    <t>log(N)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
@@ -644,6 +647,7 @@
     <numFmt numFmtId="171" formatCode="0.000E+00"/>
     <numFmt numFmtId="172" formatCode="0.000000"/>
     <numFmt numFmtId="173" formatCode="0.00000%"/>
+    <numFmt numFmtId="177" formatCode="0.0000000E+00"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -846,7 +850,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -935,6 +939,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -945,6 +952,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -977,13 +993,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2527,9 +2537,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11005314960629921"/>
+          <c:x val="0.11838648293963254"/>
           <c:y val="4.9724840458721442E-2"/>
-          <c:w val="0.85749540682414693"/>
+          <c:w val="0.84916207349081352"/>
           <c:h val="0.78822521472980045"/>
         </c:manualLayout>
       </c:layout>
@@ -2563,139 +2573,132 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'P1.2'!$N$4:$N$21</c:f>
+              <c:f>'P1.2'!$P$4:$P$21</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.3</c:v>
+                  <c:v>-0.52287874528033762</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4</c:v>
+                  <c:v>-0.3979400086720376</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>-0.3010299956639812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6</c:v>
+                  <c:v>-0.22184874961635639</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7</c:v>
+                  <c:v>-0.15490195998574319</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8</c:v>
+                  <c:v>-9.6910013008056392E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9</c:v>
+                  <c:v>-4.5757490560675115E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>4.1392685158225077E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2</c:v>
+                  <c:v>7.9181246047624818E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3</c:v>
+                  <c:v>0.11394335230683679</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.4</c:v>
+                  <c:v>0.14612803567823801</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.5</c:v>
+                  <c:v>0.17609125905568124</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.6</c:v>
+                  <c:v>0.20411998265592479</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.7</c:v>
+                  <c:v>0.23044892137827391</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.8</c:v>
+                  <c:v>0.25527250510330607</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.9</c:v>
+                  <c:v>0.27875360095282892</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2</c:v>
+                  <c:v>0.3010299956639812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'P1.2'!$O$4:$O$21</c:f>
+              <c:f>'P1.2'!$Q$4:$Q$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0.69897000433601886</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>0.90308998699194354</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>1.0791812460476249</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>1.146128035678238</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>1.2041199826559248</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18</c:v>
+                  <c:v>1.255272505103306</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>1.3222192947339193</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22</c:v>
+                  <c:v>1.3424226808222062</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24</c:v>
+                  <c:v>1.3802112417116059</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27</c:v>
+                  <c:v>1.4313637641589874</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30</c:v>
+                  <c:v>1.4771212547196624</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>33</c:v>
+                  <c:v>1.5185139398778875</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35</c:v>
+                  <c:v>1.5440680443502757</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>38</c:v>
+                  <c:v>1.5797835966168101</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>39</c:v>
+                  <c:v>1.5910646070264991</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>42</c:v>
+                  <c:v>1.6232492903979006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>45</c:v>
+                  <c:v>1.6532125137753437</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:filteredSeriesTitle>
-                <c15:tx>
-                  <c:v>N(p)</c:v>
-                </c15:tx>
-              </c15:filteredSeriesTitle>
-            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-49EE-4463-99F7-959DF4B2D737}"/>
             </c:ext>
@@ -2719,19 +2722,7 @@
           <c:dPt>
             <c:idx val="0"/>
             <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent3"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
+              <c:symbol val="none"/>
             </c:marker>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -2742,139 +2733,132 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>'P1.2'!$N$4:$N$21</c:f>
+              <c:f>'P1.2'!$P$4:$P$21</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.3</c:v>
+                  <c:v>-0.52287874528033762</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4</c:v>
+                  <c:v>-0.3979400086720376</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>-0.3010299956639812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6</c:v>
+                  <c:v>-0.22184874961635639</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7</c:v>
+                  <c:v>-0.15490195998574319</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8</c:v>
+                  <c:v>-9.6910013008056392E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9</c:v>
+                  <c:v>-4.5757490560675115E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>4.1392685158225077E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2</c:v>
+                  <c:v>7.9181246047624818E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3</c:v>
+                  <c:v>0.11394335230683679</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.4</c:v>
+                  <c:v>0.14612803567823801</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.5</c:v>
+                  <c:v>0.17609125905568124</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.6</c:v>
+                  <c:v>0.20411998265592479</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.7</c:v>
+                  <c:v>0.23044892137827391</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.8</c:v>
+                  <c:v>0.25527250510330607</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.9</c:v>
+                  <c:v>0.27875360095282892</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2</c:v>
+                  <c:v>0.3010299956639812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'P1.2'!$P$4:$P$21</c:f>
+              <c:f>'P1.2'!$R$4:$R$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>4.730994152046792</c:v>
+                  <c:v>0.73467587300166037</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0436876504988035</c:v>
+                  <c:v>0.87315071951310141</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.3563811489508151</c:v>
+                  <c:v>0.98056015505737637</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.669074647402827</c:v>
+                  <c:v>1.0683200539541056</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.981768145854836</c:v>
+                  <c:v>1.1425199912209358</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.29446164430685</c:v>
+                  <c:v>1.2067949004655465</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18.607155142758863</c:v>
+                  <c:v>1.2634893883951099</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.919848641210873</c:v>
+                  <c:v>1.3142043360098217</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23.232542139662886</c:v>
+                  <c:v>1.3600815865694438</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25.545235638114896</c:v>
+                  <c:v>1.4019642349065509</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.857929136566909</c:v>
+                  <c:v>1.4404925365312928</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30.170622635018916</c:v>
+                  <c:v>1.4761641721733811</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>32.483316133470929</c:v>
+                  <c:v>1.509373670450826</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34.796009631922942</c:v>
+                  <c:v>1.5404390814179918</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>37.108703130374955</c:v>
+                  <c:v>1.5696205494507351</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>39.421396628826969</c:v>
+                  <c:v>1.5971335693475552</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41.734090127278975</c:v>
+                  <c:v>1.6231586535764533</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44.046783625730988</c:v>
+                  <c:v>1.647848516962267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:filteredSeriesTitle>
-                <c15:tx>
-                  <c:v>ajuste</c:v>
-                </c15:tx>
-              </c15:filteredSeriesTitle>
-            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-49EE-4463-99F7-959DF4B2D737}"/>
             </c:ext>
@@ -2933,7 +2917,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>p (bar)</a:t>
+                  <a:t>log(p) (s.u.)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2967,7 +2951,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3050,7 +3034,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>N (s.u.)</a:t>
+                  <a:t>log(N) (s.u.)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3122,7 +3106,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1010304288"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="-2222"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3289,126 +3273,126 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'P1.2'!$N$4:$N$21</c:f>
+              <c:f>'P1.2'!$P$4:$P$21</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.3</c:v>
+                  <c:v>-0.52287874528033762</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4</c:v>
+                  <c:v>-0.3979400086720376</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>-0.3010299956639812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6</c:v>
+                  <c:v>-0.22184874961635639</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7</c:v>
+                  <c:v>-0.15490195998574319</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8</c:v>
+                  <c:v>-9.6910013008056392E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9</c:v>
+                  <c:v>-4.5757490560675115E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>4.1392685158225077E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2</c:v>
+                  <c:v>7.9181246047624818E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3</c:v>
+                  <c:v>0.11394335230683679</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.4</c:v>
+                  <c:v>0.14612803567823801</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.5</c:v>
+                  <c:v>0.17609125905568124</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.6</c:v>
+                  <c:v>0.20411998265592479</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.7</c:v>
+                  <c:v>0.23044892137827391</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.8</c:v>
+                  <c:v>0.25527250510330607</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.9</c:v>
+                  <c:v>0.27875360095282892</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2</c:v>
+                  <c:v>0.3010299956639812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'P1.2'!$Q$4:$Q$21</c:f>
+              <c:f>'P1.2'!$S$4:$S$21</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.26900584795320803</c:v>
+                  <c:v>-3.5705868665641516E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95631234950119648</c:v>
+                  <c:v>2.9939267478842124E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.64361885104918493</c:v>
+                  <c:v>1.943984494262363E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.33092535259717337</c:v>
+                  <c:v>1.0861192093519323E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8231854145163595E-2</c:v>
+                  <c:v>3.6080444573021175E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.29446164430684973</c:v>
+                  <c:v>-2.6749178096217019E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.60715514275886306</c:v>
+                  <c:v>-8.2168832918039225E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0151358789127158E-2</c:v>
+                  <c:v>8.0149587240976317E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.2325421396628862</c:v>
+                  <c:v>-1.7658905747237608E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.5452356381148959</c:v>
+                  <c:v>-2.1752993194944947E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.85792913656690928</c:v>
+                  <c:v>-9.1287723723054714E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.1706226350189155</c:v>
+                  <c:v>9.5708254628124045E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.51668386652907117</c:v>
+                  <c:v>9.1402694270614759E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.20399036807705784</c:v>
+                  <c:v>3.6289629322838746E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.89129686962504451</c:v>
+                  <c:v>1.0163047166074968E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.42139662882696882</c:v>
+                  <c:v>-6.0689623210561372E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.26590987272102495</c:v>
+                  <c:v>9.0636821447276361E-5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.95321637426901162</c:v>
+                  <c:v>5.3639968130767546E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3473,7 +3457,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>p (bar)</a:t>
+                  <a:t>log(p) (s.u.)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3507,7 +3491,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3590,7 +3574,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>N-N</a:t>
+                  <a:t>log(N)-log(N)</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400" baseline="-25000"/>
@@ -3632,7 +3616,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3670,7 +3654,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="729533424"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="-20"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -10801,13 +10785,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>30</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>60960</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>472440</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>148536</xdr:rowOff>
@@ -10881,13 +10865,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>441960</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>148590</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>137160</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>148590</xdr:rowOff>
@@ -10919,16 +10903,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>270344</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>316064</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>109496</xdr:rowOff>
+      <xdr:rowOff>94256</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>575144</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>11264</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>109496</xdr:rowOff>
+      <xdr:rowOff>94256</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11696,8 +11680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0D8ADF-2EFB-452A-A480-0B215EA5BBF1}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11713,40 +11697,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
@@ -11977,6 +11961,10 @@
       <c r="N10" s="15">
         <f>_xlfn.STDEV.P(B5:K5)/SQRT(10)</f>
         <v>1.8891797161731345E-7</v>
+      </c>
+      <c r="O10" s="30">
+        <f>N10/N9</f>
+        <v>1.7004317877345947E-2</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
@@ -12140,107 +12128,111 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A1DA6F-08FA-487A-82B4-E9BF2212A846}">
-  <dimension ref="A1:AM26"/>
+  <dimension ref="A1:AO23"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+    <sheetView topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC26" sqref="AC26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="10" width="8.88671875" style="1"/>
     <col min="11" max="11" width="12.21875" style="1" customWidth="1"/>
-    <col min="12" max="27" width="8.88671875" style="1"/>
-    <col min="28" max="28" width="13" style="1" customWidth="1"/>
-    <col min="29" max="29" width="8.88671875" style="1" customWidth="1"/>
-    <col min="30" max="16384" width="8.88671875" style="1"/>
+    <col min="12" max="29" width="8.88671875" style="1"/>
+    <col min="30" max="30" width="13" style="1" customWidth="1"/>
+    <col min="31" max="31" width="8.88671875" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
     </row>
-    <row r="2" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30"/>
-      <c r="AG2" s="30"/>
-      <c r="AH2" s="30"/>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="30"/>
-      <c r="AK2" s="30"/>
-      <c r="AL2" s="30"/>
-      <c r="AM2" s="30"/>
+    <row r="2" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
+      <c r="AF2" s="31"/>
+      <c r="AG2" s="31"/>
+      <c r="AH2" s="31"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -12260,46 +12252,52 @@
         <v>5</v>
       </c>
       <c r="P3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AC3" s="3">
+      <c r="AE3" s="3">
         <v>19</v>
       </c>
-      <c r="AD3" s="3">
+      <c r="AF3" s="3">
         <v>23</v>
       </c>
-      <c r="AE3" s="3">
+      <c r="AG3" s="3">
         <v>21</v>
       </c>
-      <c r="AF3" s="3">
+      <c r="AH3" s="3">
         <v>18</v>
       </c>
-      <c r="AG3" s="3">
+      <c r="AI3" s="3">
         <v>20</v>
       </c>
-      <c r="AH3" s="3">
+      <c r="AJ3" s="3">
         <v>20</v>
       </c>
-      <c r="AI3" s="3">
+      <c r="AK3" s="3">
         <v>21</v>
-      </c>
-      <c r="AJ3" s="3">
-        <v>21</v>
-      </c>
-      <c r="AK3" s="3">
-        <v>22</v>
       </c>
       <c r="AL3" s="3">
         <v>21</v>
       </c>
+      <c r="AM3" s="3">
+        <v>22</v>
+      </c>
+      <c r="AN3" s="3">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>0.3</v>
       </c>
@@ -12320,16 +12318,24 @@
       <c r="O4" s="3">
         <v>5</v>
       </c>
-      <c r="P4" s="8">
-        <f t="shared" ref="P4:P21" si="1">N4*T$21+U$21</f>
-        <v>4.730994152046792</v>
-      </c>
-      <c r="Q4" s="8">
-        <f>O4-P4</f>
-        <v>0.26900584795320803</v>
+      <c r="P4" s="3">
+        <f>LOG(N4)</f>
+        <v>-0.52287874528033762</v>
+      </c>
+      <c r="Q4" s="3">
+        <f>LOG(O4)</f>
+        <v>0.69897000433601886</v>
+      </c>
+      <c r="R4" s="8">
+        <f t="shared" ref="R4:R21" si="1">P4*V$21+W$21</f>
+        <v>0.73467587300166037</v>
+      </c>
+      <c r="S4" s="9">
+        <f>Q4-R4</f>
+        <v>-3.5705868665641516E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>0.4</v>
       </c>
@@ -12350,23 +12356,31 @@
       <c r="O5" s="3">
         <v>8</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="3">
+        <f t="shared" ref="P5:P21" si="3">LOG(N5)</f>
+        <v>-0.3979400086720376</v>
+      </c>
+      <c r="Q5" s="3">
+        <f t="shared" ref="Q5:Q21" si="4">LOG(O5)</f>
+        <v>0.90308998699194354</v>
+      </c>
+      <c r="R5" s="8">
         <f t="shared" si="1"/>
-        <v>7.0436876504988035</v>
-      </c>
-      <c r="Q5" s="8">
-        <f t="shared" ref="Q5:Q21" si="3">O5-P5</f>
-        <v>0.95631234950119648</v>
-      </c>
-      <c r="AB5" s="2" t="s">
+        <v>0.87315071951310141</v>
+      </c>
+      <c r="S5" s="9">
+        <f t="shared" ref="S5:S21" si="5">Q5-R5</f>
+        <v>2.9939267478842124E-2</v>
+      </c>
+      <c r="AD5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AC5" s="3">
-        <f>AVERAGE(AC3:AL3)</f>
+      <c r="AE5" s="3">
+        <f>AVERAGE(AE3:AN3)</f>
         <v>20.6</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>0.5</v>
       </c>
@@ -12387,23 +12401,31 @@
       <c r="O6" s="3">
         <v>10</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.3010299956639812</v>
+      </c>
+      <c r="Q6" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="R6" s="8">
         <f t="shared" si="1"/>
-        <v>9.3563811489508151</v>
-      </c>
-      <c r="Q6" s="8">
-        <f t="shared" si="3"/>
-        <v>0.64361885104918493</v>
-      </c>
-      <c r="AB6" s="2" t="s">
+        <v>0.98056015505737637</v>
+      </c>
+      <c r="S6" s="9">
+        <f t="shared" si="5"/>
+        <v>1.943984494262363E-2</v>
+      </c>
+      <c r="AD6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AC6" s="13">
-        <f>_xlfn.STDEV.P(AC3:AL3)/SQRT(COUNTA(AC3:AL3))</f>
+      <c r="AE6" s="13">
+        <f>_xlfn.STDEV.P(AE3:AN3)/SQRT(COUNTA(AE3:AN3))</f>
         <v>0.42895221179054438</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>0.6</v>
       </c>
@@ -12424,23 +12446,31 @@
       <c r="O7" s="3">
         <v>12</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.22184874961635639</v>
+      </c>
+      <c r="Q7" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0791812460476249</v>
+      </c>
+      <c r="R7" s="8">
         <f t="shared" si="1"/>
-        <v>11.669074647402827</v>
-      </c>
-      <c r="Q7" s="8">
-        <f t="shared" si="3"/>
-        <v>0.33092535259717337</v>
-      </c>
-      <c r="AB7" s="2" t="s">
+        <v>1.0683200539541056</v>
+      </c>
+      <c r="S7" s="9">
+        <f t="shared" si="5"/>
+        <v>1.0861192093519323E-2</v>
+      </c>
+      <c r="AD7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AC7" s="19">
-        <f>1 + ($L$20*AC5)/(2*$L$22)</f>
+      <c r="AE7" s="19">
+        <f>1 + ($L$20*AE5)/(2*$L$22)</f>
         <v>1.0002172613333333</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>0.7</v>
       </c>
@@ -12461,23 +12491,31 @@
       <c r="O8" s="3">
         <v>14</v>
       </c>
-      <c r="P8" s="8">
+      <c r="P8" s="3">
+        <f t="shared" si="3"/>
+        <v>-0.15490195998574319</v>
+      </c>
+      <c r="Q8" s="3">
+        <f t="shared" si="4"/>
+        <v>1.146128035678238</v>
+      </c>
+      <c r="R8" s="8">
         <f t="shared" si="1"/>
-        <v>13.981768145854836</v>
-      </c>
-      <c r="Q8" s="8">
-        <f t="shared" si="3"/>
-        <v>1.8231854145163595E-2</v>
-      </c>
-      <c r="AB8" s="2" t="s">
+        <v>1.1425199912209358</v>
+      </c>
+      <c r="S8" s="9">
+        <f t="shared" si="5"/>
+        <v>3.6080444573021175E-3</v>
+      </c>
+      <c r="AD8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AC8" s="19">
-        <f>SQRT((L20*2/((2*L22)^2)*L22*AC6)^2 + (L20*2/((2*L22)^2)*AC5*L23)^2)</f>
+      <c r="AE8" s="19">
+        <f>SQRT((L20*2/((2*L22)^2)*L22*AE6)^2 + (L20*2/((2*L22)^2)*AE5*L23)^2)</f>
         <v>8.5389653030340718E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>0.8</v>
       </c>
@@ -12498,23 +12536,31 @@
       <c r="O9" s="3">
         <v>16</v>
       </c>
-      <c r="P9" s="8">
+      <c r="P9" s="3">
+        <f t="shared" si="3"/>
+        <v>-9.6910013008056392E-2</v>
+      </c>
+      <c r="Q9" s="3">
+        <f t="shared" si="4"/>
+        <v>1.2041199826559248</v>
+      </c>
+      <c r="R9" s="8">
         <f t="shared" si="1"/>
-        <v>16.29446164430685</v>
-      </c>
-      <c r="Q9" s="8">
-        <f t="shared" si="3"/>
-        <v>-0.29446164430684973</v>
-      </c>
-      <c r="AB9" s="2" t="s">
+        <v>1.2067949004655465</v>
+      </c>
+      <c r="S9" s="9">
+        <f t="shared" si="5"/>
+        <v>-2.6749178096217019E-3</v>
+      </c>
+      <c r="AD9" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AC9" s="20">
-        <f>AC8/AC7</f>
+      <c r="AE9" s="20">
+        <f>AE8/AE7</f>
         <v>8.5371105190198948E-6</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>0.9</v>
       </c>
@@ -12535,23 +12581,31 @@
       <c r="O10" s="3">
         <v>18</v>
       </c>
-      <c r="P10" s="8">
+      <c r="P10" s="3">
+        <f t="shared" si="3"/>
+        <v>-4.5757490560675115E-2</v>
+      </c>
+      <c r="Q10" s="3">
+        <f t="shared" si="4"/>
+        <v>1.255272505103306</v>
+      </c>
+      <c r="R10" s="8">
         <f t="shared" si="1"/>
-        <v>18.607155142758863</v>
-      </c>
-      <c r="Q10" s="8">
-        <f t="shared" si="3"/>
-        <v>-0.60715514275886306</v>
-      </c>
-      <c r="AB10" s="2" t="s">
+        <v>1.2634893883951099</v>
+      </c>
+      <c r="S10" s="9">
+        <f t="shared" si="5"/>
+        <v>-8.2168832918039225E-3</v>
+      </c>
+      <c r="AD10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AC10" s="11">
-        <f>ABS(AC7-L21)/L21</f>
+      <c r="AE10" s="11">
+        <f>ABS(AE7-L21)/L21</f>
         <v>7.2717578568786971E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -12572,16 +12626,24 @@
       <c r="O11" s="3">
         <v>21</v>
       </c>
-      <c r="P11" s="8">
+      <c r="P11" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3">
+        <f t="shared" si="4"/>
+        <v>1.3222192947339193</v>
+      </c>
+      <c r="R11" s="8">
         <f t="shared" si="1"/>
-        <v>20.919848641210873</v>
-      </c>
-      <c r="Q11" s="8">
-        <f t="shared" si="3"/>
-        <v>8.0151358789127158E-2</v>
+        <v>1.3142043360098217</v>
+      </c>
+      <c r="S11" s="9">
+        <f t="shared" si="5"/>
+        <v>8.0149587240976317E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>1.1000000000000001</v>
       </c>
@@ -12602,16 +12664,24 @@
       <c r="O12" s="3">
         <v>22</v>
       </c>
-      <c r="P12" s="8">
+      <c r="P12" s="3">
+        <f t="shared" si="3"/>
+        <v>4.1392685158225077E-2</v>
+      </c>
+      <c r="Q12" s="3">
+        <f t="shared" si="4"/>
+        <v>1.3424226808222062</v>
+      </c>
+      <c r="R12" s="8">
         <f t="shared" si="1"/>
-        <v>23.232542139662886</v>
-      </c>
-      <c r="Q12" s="8">
-        <f t="shared" si="3"/>
-        <v>-1.2325421396628862</v>
+        <v>1.3600815865694438</v>
+      </c>
+      <c r="S12" s="9">
+        <f t="shared" si="5"/>
+        <v>-1.7658905747237608E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>1.3</v>
       </c>
@@ -12632,16 +12702,24 @@
       <c r="O13" s="3">
         <v>24</v>
       </c>
-      <c r="P13" s="8">
+      <c r="P13" s="3">
+        <f t="shared" si="3"/>
+        <v>7.9181246047624818E-2</v>
+      </c>
+      <c r="Q13" s="3">
+        <f t="shared" si="4"/>
+        <v>1.3802112417116059</v>
+      </c>
+      <c r="R13" s="8">
         <f t="shared" si="1"/>
-        <v>25.545235638114896</v>
-      </c>
-      <c r="Q13" s="8">
-        <f t="shared" si="3"/>
-        <v>-1.5452356381148959</v>
+        <v>1.4019642349065509</v>
+      </c>
+      <c r="S13" s="9">
+        <f t="shared" si="5"/>
+        <v>-2.1752993194944947E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>1.5</v>
       </c>
@@ -12662,16 +12740,24 @@
       <c r="O14" s="3">
         <v>27</v>
       </c>
-      <c r="P14" s="8">
+      <c r="P14" s="3">
+        <f t="shared" si="3"/>
+        <v>0.11394335230683679</v>
+      </c>
+      <c r="Q14" s="3">
+        <f t="shared" si="4"/>
+        <v>1.4313637641589874</v>
+      </c>
+      <c r="R14" s="8">
         <f t="shared" si="1"/>
-        <v>27.857929136566909</v>
-      </c>
-      <c r="Q14" s="8">
-        <f t="shared" si="3"/>
-        <v>-0.85792913656690928</v>
+        <v>1.4404925365312928</v>
+      </c>
+      <c r="S14" s="9">
+        <f t="shared" si="5"/>
+        <v>-9.1287723723054714E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>1.7</v>
       </c>
@@ -12692,16 +12778,24 @@
       <c r="O15" s="3">
         <v>30</v>
       </c>
-      <c r="P15" s="8">
+      <c r="P15" s="3">
+        <f t="shared" si="3"/>
+        <v>0.14612803567823801</v>
+      </c>
+      <c r="Q15" s="3">
+        <f t="shared" si="4"/>
+        <v>1.4771212547196624</v>
+      </c>
+      <c r="R15" s="8">
         <f t="shared" si="1"/>
-        <v>30.170622635018916</v>
-      </c>
-      <c r="Q15" s="8">
-        <f t="shared" si="3"/>
-        <v>-0.1706226350189155</v>
+        <v>1.4761641721733811</v>
+      </c>
+      <c r="S15" s="9">
+        <f t="shared" si="5"/>
+        <v>9.5708254628124045E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>1.8</v>
       </c>
@@ -12722,16 +12816,24 @@
       <c r="O16" s="3">
         <v>33</v>
       </c>
-      <c r="P16" s="8">
+      <c r="P16" s="3">
+        <f t="shared" si="3"/>
+        <v>0.17609125905568124</v>
+      </c>
+      <c r="Q16" s="3">
+        <f t="shared" si="4"/>
+        <v>1.5185139398778875</v>
+      </c>
+      <c r="R16" s="8">
         <f t="shared" si="1"/>
-        <v>32.483316133470929</v>
-      </c>
-      <c r="Q16" s="8">
-        <f t="shared" si="3"/>
-        <v>0.51668386652907117</v>
+        <v>1.509373670450826</v>
+      </c>
+      <c r="S16" s="9">
+        <f t="shared" si="5"/>
+        <v>9.1402694270614759E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>1.85</v>
       </c>
@@ -12752,16 +12854,24 @@
       <c r="O17" s="3">
         <v>35</v>
       </c>
-      <c r="P17" s="8">
+      <c r="P17" s="3">
+        <f t="shared" si="3"/>
+        <v>0.20411998265592479</v>
+      </c>
+      <c r="Q17" s="3">
+        <f t="shared" si="4"/>
+        <v>1.5440680443502757</v>
+      </c>
+      <c r="R17" s="8">
         <f t="shared" si="1"/>
-        <v>34.796009631922942</v>
-      </c>
-      <c r="Q17" s="8">
-        <f t="shared" si="3"/>
-        <v>0.20399036807705784</v>
+        <v>1.5404390814179918</v>
+      </c>
+      <c r="S17" s="9">
+        <f t="shared" si="5"/>
+        <v>3.6289629322838746E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>1.92</v>
       </c>
@@ -12782,16 +12892,24 @@
       <c r="O18" s="3">
         <v>38</v>
       </c>
-      <c r="P18" s="8">
+      <c r="P18" s="3">
+        <f t="shared" si="3"/>
+        <v>0.23044892137827391</v>
+      </c>
+      <c r="Q18" s="3">
+        <f t="shared" si="4"/>
+        <v>1.5797835966168101</v>
+      </c>
+      <c r="R18" s="8">
         <f t="shared" si="1"/>
-        <v>37.108703130374955</v>
-      </c>
-      <c r="Q18" s="8">
-        <f t="shared" si="3"/>
-        <v>0.89129686962504451</v>
+        <v>1.5696205494507351</v>
+      </c>
+      <c r="S18" s="9">
+        <f t="shared" si="5"/>
+        <v>1.0163047166074968E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>1.98</v>
       </c>
@@ -12812,22 +12930,30 @@
       <c r="O19" s="3">
         <v>39</v>
       </c>
-      <c r="P19" s="8">
+      <c r="P19" s="3">
+        <f t="shared" si="3"/>
+        <v>0.25527250510330607</v>
+      </c>
+      <c r="Q19" s="3">
+        <f t="shared" si="4"/>
+        <v>1.5910646070264991</v>
+      </c>
+      <c r="R19" s="8">
         <f t="shared" si="1"/>
-        <v>39.421396628826969</v>
-      </c>
-      <c r="Q19" s="8">
-        <f t="shared" si="3"/>
-        <v>-0.42139662882696882</v>
+        <v>1.5971335693475552</v>
+      </c>
+      <c r="S19" s="9">
+        <f t="shared" si="5"/>
+        <v>-6.0689623210561372E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="F20" s="31" t="s">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="F20" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
       <c r="K20" s="2" t="s">
         <v>19</v>
       </c>
@@ -12840,22 +12966,30 @@
       <c r="O20" s="3">
         <v>42</v>
       </c>
-      <c r="P20" s="8">
+      <c r="P20" s="3">
+        <f t="shared" si="3"/>
+        <v>0.27875360095282892</v>
+      </c>
+      <c r="Q20" s="3">
+        <f t="shared" si="4"/>
+        <v>1.6232492903979006</v>
+      </c>
+      <c r="R20" s="8">
         <f t="shared" si="1"/>
-        <v>41.734090127278975</v>
-      </c>
-      <c r="Q20" s="8">
-        <f t="shared" si="3"/>
-        <v>0.26590987272102495</v>
-      </c>
-      <c r="S20" s="31" t="s">
+        <v>1.6231586535764533</v>
+      </c>
+      <c r="S20" s="9">
+        <f t="shared" si="5"/>
+        <v>9.0636821447276361E-5</v>
+      </c>
+      <c r="U20" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="T20" s="31"/>
-      <c r="U20" s="31"/>
-      <c r="V20" s="31"/>
+      <c r="V20" s="32"/>
+      <c r="W20" s="32"/>
+      <c r="X20" s="32"/>
     </row>
-    <row r="21" spans="1:27" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" ht="15" x14ac:dyDescent="0.3">
       <c r="F21" s="2" t="s">
         <v>26</v>
       </c>
@@ -12881,29 +13015,41 @@
       <c r="O21" s="3">
         <v>45</v>
       </c>
-      <c r="P21" s="8">
+      <c r="P21" s="3">
+        <f t="shared" si="3"/>
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="Q21" s="3">
+        <f t="shared" si="4"/>
+        <v>1.6532125137753437</v>
+      </c>
+      <c r="R21" s="8">
         <f t="shared" si="1"/>
-        <v>44.046783625730988</v>
-      </c>
-      <c r="Q21" s="8">
-        <f t="shared" si="3"/>
-        <v>0.95321637426901162</v>
-      </c>
-      <c r="S21" s="2" t="s">
+        <v>1.647848516962267</v>
+      </c>
+      <c r="S21" s="9">
+        <f t="shared" si="5"/>
+        <v>5.3639968130767546E-3</v>
+      </c>
+      <c r="U21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T21" s="13">
-        <f t="array" ref="T21:U23">LINEST(O4:O21,N4:N21,1,1)</f>
-        <v>23.126934984520116</v>
-      </c>
-      <c r="U21" s="13">
-        <v>-2.2070863433092427</v>
-      </c>
-      <c r="V21" s="2" t="s">
+      <c r="V21" s="8">
+        <f t="array" ref="V21:W23">LINEST(Q4:Q21,P4:P21,1,1)</f>
+        <v>1.1083419784016109</v>
+      </c>
+      <c r="W21" s="9">
+        <v>1.3142043360098217</v>
+      </c>
+      <c r="X21" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="Y21" s="30">
+        <f>V22/V21</f>
+        <v>1.412527374797384E-2</v>
+      </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="F22" s="2" t="s">
         <v>27</v>
       </c>
@@ -12922,22 +13068,26 @@
       <c r="L22" s="3">
         <v>0.03</v>
       </c>
-      <c r="S22" s="2" t="s">
+      <c r="U22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="T22" s="13">
-        <v>0.33892458700223815</v>
-      </c>
-      <c r="U22" s="13">
-        <v>0.42759157161415734</v>
-      </c>
-      <c r="V22" s="2" t="s">
+      <c r="V22" s="8">
+        <v>1.5655633851293663E-2</v>
+      </c>
+      <c r="W22" s="9">
+        <v>3.7060123412108389E-3</v>
+      </c>
+      <c r="X22" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="Y22" s="30">
+        <f>(1-V21)/1</f>
+        <v>-0.10834197840161086</v>
+      </c>
     </row>
-    <row r="23" spans="1:27" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" ht="16.2" x14ac:dyDescent="0.3">
       <c r="F23" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G23" s="9">
         <v>0.99274932078895828</v>
@@ -12954,29 +13104,24 @@
       <c r="L23" s="3">
         <v>1E-3</v>
       </c>
-      <c r="S23" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="T23" s="9">
-        <v>0.99657547634395116</v>
-      </c>
-      <c r="U23" s="13">
-        <v>0.74601913356402572</v>
-      </c>
-      <c r="V23" s="2" t="s">
+      <c r="U23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="V23" s="9">
+        <v>0.99681778508403462</v>
+      </c>
+      <c r="W23" s="8">
+        <v>1.5720142982837994E-2</v>
+      </c>
+      <c r="X23" s="2" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="AA26" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="F20:I20"/>
-    <mergeCell ref="S20:V20"/>
-    <mergeCell ref="A1:AM2"/>
+    <mergeCell ref="U20:X20"/>
+    <mergeCell ref="A1:AO2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12988,7 +13133,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13004,42 +13149,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
     </row>
     <row r="3" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -13125,20 +13270,20 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="32"/>
+      <c r="C10" s="33"/>
       <c r="D10" s="9">
         <f>AVERAGE(D4:D9)</f>
         <v>1.3986112703403737</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="32"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="9">
         <f>_xlfn.STDEV.P(D4:D9)/SQRT(6)</f>
         <v>1.7248884176812387E-2</v>
@@ -13151,10 +13296,10 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="32"/>
+      <c r="C12" s="33"/>
       <c r="D12" s="6">
         <f>D11/D10</f>
         <v>1.2332865137440658E-2</v>
@@ -13167,10 +13312,10 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="32"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="6">
         <f>ABS(D10-G15)/G15</f>
         <v>7.8041351126978395E-2</v>
@@ -13280,40 +13425,40 @@
       </c>
     </row>
     <row r="22" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="33"/>
+      <c r="C22" s="34"/>
       <c r="D22" s="24">
         <f>AVERAGE(D16:D21)</f>
         <v>1.385930248013185</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="33"/>
+      <c r="C23" s="34"/>
       <c r="D23" s="24">
         <f>_xlfn.STDEV.P(D16:D21)/SQRT(6)</f>
         <v>9.7844189204701823E-3</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="33"/>
+      <c r="C24" s="34"/>
       <c r="D24" s="25">
         <f>D23/D22</f>
         <v>7.0598206038844594E-3</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="33"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="25">
         <f>ABS(D22-G15)/G15</f>
         <v>8.640062754569211E-2</v>
@@ -13341,14 +13486,14 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="8.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
     <col min="6" max="9" width="8.88671875" style="1"/>
@@ -13357,40 +13502,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
     </row>
     <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -13410,7 +13555,7 @@
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="48">
         <f>ABS(B4)*K$6*K$4/(K$5*A4)</f>
         <v>1.5582344278054102E-4</v>
       </c>
@@ -13428,8 +13573,8 @@
       <c r="B5" s="3">
         <v>-1</v>
       </c>
-      <c r="C5" s="4">
-        <f t="shared" ref="C5:C11" si="0">ABS(B5)*K$6*K$4/(K$5*A5)</f>
+      <c r="C5" s="48">
+        <f>ABS(B5)*K$6*K$4/(K$5*A5)</f>
         <v>1.6448030071279331E-4</v>
       </c>
       <c r="J5" s="5" t="s">
@@ -13446,8 +13591,8 @@
       <c r="B6" s="3">
         <v>2</v>
       </c>
-      <c r="C6" s="4">
-        <f t="shared" si="0"/>
+      <c r="C6" s="48">
+        <f t="shared" ref="C5:C11" si="0">ABS(B6)*K$6*K$4/(K$5*A6)</f>
         <v>1.7415561251942819E-4</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -13464,8 +13609,8 @@
       <c r="B7" s="3">
         <v>-2</v>
       </c>
-      <c r="C7" s="4">
-        <f t="shared" si="0"/>
+      <c r="C7" s="48">
+        <f>ABS(B7)*K$6*K$4/(K$5*A7)</f>
         <v>1.6448030071279331E-4</v>
       </c>
       <c r="J7" s="2" t="s">
@@ -13482,7 +13627,7 @@
       <c r="B8" s="3">
         <v>3</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="48">
         <f t="shared" si="0"/>
         <v>1.7415561251942819E-4</v>
       </c>
@@ -13500,7 +13645,7 @@
       <c r="B9" s="3">
         <v>-3</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="48">
         <f t="shared" si="0"/>
         <v>1.6448030071279329E-4</v>
       </c>
@@ -13512,7 +13657,7 @@
       <c r="B10" s="3">
         <v>4</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="48">
         <f t="shared" si="0"/>
         <v>1.6917973787601595E-4</v>
       </c>
@@ -13524,46 +13669,46 @@
       <c r="B11" s="3">
         <v>-4</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="48">
         <f t="shared" si="0"/>
         <v>1.6448030071279331E-4</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="32"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="4">
         <f>AVERAGE(C4:C11)</f>
         <v>1.6640445106832331E-4</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="32"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="15">
         <f>_xlfn.STDEV.P(C4:C11)/SQRT(COUNTA(C4:C11))</f>
         <v>1.9946427440772595E-6</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="32"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="6">
         <f>C13/C12</f>
         <v>1.1986715086474985E-2</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="32"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="6">
         <f>ABS(C12-K8)/K8</f>
         <v>4.0027819177020571E-2</v>
@@ -13588,7 +13733,8 @@
     <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -13597,7 +13743,7 @@
   <dimension ref="B1:P9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13608,40 +13754,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" s="26" t="s">
@@ -13671,13 +13817,17 @@
         <f>ABS(C4)*L$6*L$4/(L$5*B4)</f>
         <v>5.9491259534734934E-5</v>
       </c>
-      <c r="E4" s="44">
+      <c r="E4" s="35">
         <f>AVERAGE(D4:D11)</f>
         <v>6.3111098077853726E-5</v>
       </c>
-      <c r="F4" s="44">
+      <c r="F4" s="35">
         <f>_xlfn.STDEV.P(D4:D11)/SQRT(COUNTA(D4:D11))</f>
         <v>1.1165783691493025E-6</v>
+      </c>
+      <c r="G4" s="30">
+        <f>F4/E4</f>
+        <v>1.7692266545131154E-2</v>
       </c>
       <c r="K4" s="26" t="s">
         <v>19</v>
@@ -13697,8 +13847,8 @@
         <f t="shared" ref="D5:D9" si="0">ABS(C5)*L$6*L$4/(L$5*B5)</f>
         <v>5.9491259534734934E-5</v>
       </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
       <c r="K5" s="29" t="s">
         <v>50</v>
       </c>
@@ -13717,8 +13867,8 @@
         <f t="shared" si="0"/>
         <v>6.6101399483038822E-5</v>
       </c>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="K6" s="26" t="s">
         <v>37</v>
       </c>
@@ -13737,8 +13887,8 @@
         <f t="shared" si="0"/>
         <v>6.6101399483038822E-5</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
       <c r="K7" s="26" t="s">
         <v>38</v>
       </c>
@@ -13757,8 +13907,8 @@
         <f t="shared" si="0"/>
         <v>6.3740635215787423E-5</v>
       </c>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="27">
@@ -13771,8 +13921,8 @@
         <f t="shared" si="0"/>
         <v>6.3740635215787423E-5</v>
       </c>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
       <c r="H9" s="1" t="s">
         <v>83</v>
       </c>
@@ -13784,7 +13934,8 @@
     <mergeCell ref="E4:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -13792,8 +13943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D173081-7852-47E0-A7A6-CA8790E2233F}">
   <dimension ref="B1:X19"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13806,56 +13957,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
     </row>
     <row r="2" spans="2:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
@@ -13893,7 +14044,7 @@
       <c r="E10" s="4">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="43">
         <v>1.8499999999999999E-2</v>
       </c>
       <c r="M10" s="5" t="s">
@@ -13916,7 +14067,7 @@
       <c r="E11" s="4">
         <v>1.2E-2</v>
       </c>
-      <c r="F11" s="40"/>
+      <c r="F11" s="44"/>
       <c r="M11" s="2" t="s">
         <v>61</v>
       </c>
@@ -13937,7 +14088,7 @@
       <c r="E12" s="4">
         <v>1.35E-2</v>
       </c>
-      <c r="F12" s="41"/>
+      <c r="F12" s="45"/>
       <c r="M12" s="2" t="s">
         <v>62</v>
       </c>
@@ -14025,49 +14176,49 @@
       <c r="B16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="39">
         <f>AVERAGE(C15:F15)</f>
         <v>3.9466298308136718E-4</v>
       </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="37"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="41"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="38">
+      <c r="C17" s="42">
         <f>_xlfn.STDEV.P(C15:F15)/SQRT(COUNTA(C15:F15))</f>
         <v>1.7932394288441141E-5</v>
       </c>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="38">
         <f>C17/C16</f>
         <v>4.5437233936743544E-2</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="34">
+      <c r="C19" s="38">
         <f>ABS(C16-N13)/N13</f>
         <v>1.3342542296582105E-2</v>
       </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -14079,7 +14230,8 @@
     <mergeCell ref="F10:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -14088,7 +14240,7 @@
   <dimension ref="B1:P22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14099,40 +14251,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -14160,20 +14312,20 @@
       </c>
       <c r="D4" s="3">
         <f>ABS(C4)*L$6*L$4/(L$5*B4)</f>
-        <v>6.0731187955492917E-5</v>
-      </c>
-      <c r="E4" s="42">
+        <v>2.9606454128302791E-4</v>
+      </c>
+      <c r="E4" s="46">
         <f>AVERAGE(D4:D11)</f>
-        <v>3.8888126178535052E-5</v>
-      </c>
-      <c r="F4" s="42">
+        <v>1.8957961512035837E-4</v>
+      </c>
+      <c r="F4" s="46">
         <f>_xlfn.STDEV.P(D4:D11)/SQRT(COUNTA(D4:D11))</f>
-        <v>3.7376974630495201E-6</v>
-      </c>
-      <c r="H4" s="43" t="s">
+        <v>1.8221275132366407E-5</v>
+      </c>
+      <c r="H4" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="43"/>
+      <c r="I4" s="47"/>
       <c r="K4" s="2" t="s">
         <v>19</v>
       </c>
@@ -14190,12 +14342,12 @@
       </c>
       <c r="D5" s="3">
         <f t="shared" ref="D5:D11" si="0">ABS(C5)*L$6*L$4/(L$5*B5)</f>
-        <v>5.0609323296244094E-5</v>
-      </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
+        <v>2.4672045106918994E-4</v>
+      </c>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
       <c r="K5" s="5" t="s">
         <v>50</v>
       </c>
@@ -14212,17 +14364,17 @@
       </c>
       <c r="D6" s="3">
         <f t="shared" si="0"/>
-        <v>3.7956992472183071E-5</v>
-      </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+        <v>1.8504033830189247E-4</v>
+      </c>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="K6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="8">
-        <v>0.48</v>
+      <c r="L6" s="10">
+        <v>2.34</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
@@ -14234,12 +14386,12 @@
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>3.9181411584188975E-5</v>
-      </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
+        <v>1.9100938147292124E-4</v>
+      </c>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
       <c r="K7" s="2" t="s">
         <v>38</v>
       </c>
@@ -14256,10 +14408,10 @@
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>3.1412683425254956E-5</v>
-      </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
+        <v>1.5313683169811788E-4</v>
+      </c>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
@@ -14270,10 +14422,10 @@
       </c>
       <c r="D9" s="3">
         <f t="shared" si="0"/>
-        <v>3.253456497615692E-5</v>
-      </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
+        <v>1.5860600425876496E-4</v>
+      </c>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
       <c r="K9" s="1">
         <v>5</v>
       </c>
@@ -14287,10 +14439,10 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" si="0"/>
-        <v>2.948115920169559E-5</v>
-      </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
+        <v>1.43720651108266E-4</v>
+      </c>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
@@ -14301,10 +14453,10 @@
       </c>
       <c r="D11" s="3">
         <f t="shared" si="0"/>
-        <v>2.9197686517063899E-5</v>
-      </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
+        <v>1.4233872177068653E-4</v>
+      </c>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
     </row>
     <row r="22" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M22" s="1" t="s">

</xml_diff>